<commit_message>
Project Schedule For week 2
</commit_message>
<xml_diff>
--- a/Planning/CAR_Project_ Schedule.xlsx
+++ b/Planning/CAR_Project_ Schedule.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion lowestEdited="5" appName="xl" rupBuild="14420" lastEdited="6"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minaz\Desktop\CarPurchasing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minaz\Desktop\CarPurchasing\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" windowHeight="9384" yWindow="0" windowWidth="23040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName localSheetId="0" name="prevWBS">GanttChart!$A1048576</definedName>
-    <definedName localSheetId="0" name="_xlnm.Print_Area">GanttChart!$A$1:$BO$48</definedName>
-    <definedName localSheetId="0" name="_xlnm.Print_Titles">GanttChart!$4:$7</definedName>
+    <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BO$44</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
-    <definedName hidden="1" name="vertex42_copyright">"© 2006-2018 Vertex42 LLC"</definedName>
-    <definedName hidden="1" name="vertex42_id">"gantt-chart_L.xlsx"</definedName>
-    <definedName hidden="1" name="vertex42_title">"Gantt Chart Template"</definedName>
+    <definedName name="vertex42_copyright" hidden="1">"© 2006-2018 Vertex42 LLC"</definedName>
+    <definedName name="vertex42_id" hidden="1">"gantt-chart_L.xlsx"</definedName>
+    <definedName name="vertex42_title" hidden="1">"Gantt Chart Template"</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,85 +33,133 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="J7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAC7UcDbE
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAC7UcDa8
     (2019-05-01 20:37:23)
-Work Days
-Counts the number of work days, excluding the weekends (Saturday and Sunday). In the PRO version, you can customize the work week and list specific non-working days like holidays. In the PRO version, the default input is the Work Days instead of the Calendar Days.</t>
+Task Description
+Enter the name of each task and sub-task. Use indents for sub-tasks.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAC7UcDbQ
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAC7UcDbA
     (2019-05-01 20:37:23)
-Percent Complete
-Update the status of this task by entering the percent complete (between 0% and 100%).</t>
+Task Lead
+Enter the name of the Task Lead in this column.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0">
+    <comment ref="D7" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAC7UcDbU
+Predecessor Tasks    (2019-05-01 20:37:23)
+You can use this column to enter the WBS of a predecessor for reference. The PRO version uses formulas to automatically calculate the Start Date based on the Predecessor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAC7UcDa0
+    (2019-05-01 20:37:23)
+Task Start Date
+You can manually enter the Start Date for each task or use a formula to create a dependency on a Predecessor. For example, you could enter =enddate+1 to set the Start date to the next calendar day, or =WORKDAY(enddate,1) to set the Start date to the next work day (excluding weekends), where enddate is the cell reference for the End date of the Predecessor task.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAC7UcDbI
+End Date    (2019-05-01 20:37:23)
+The End Date is calculated based on the Start Date and the Calendar Days columns.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
 ID#AAAAC7UcDbM
     (2019-05-01 20:37:23)
 Duration (Calendar Days)
 The duration is the number of calendar days for the given task. The duration is calculated as the End Date minus the Start Date plus 1 day, so that a task starting and ending on the same day has a duration of 1 day.
 Note: The conditional formatting used to create the gantt chart references this column.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0">
+    <comment ref="I7" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAC7UcDbI
-End Date    (2019-05-01 20:37:23)
-The End Date is calculated based on the Start Date and the Calendar Days columns.</t>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAC7UcDbQ
+    (2019-05-01 20:37:23)
+Percent Complete
+Update the status of this task by entering the percent complete (between 0% and 100%).</t>
+        </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0">
+    <comment ref="J7" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAC7UcDa0
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======
+ID#AAAAC7UcDbE
     (2019-05-01 20:37:23)
-Task Start Date
-You can manually enter the Start Date for each task or use a formula to create a dependency on a Predecessor. For example, you could enter =enddate+1 to set the Start date to the next calendar day, or =WORKDAY(enddate,1) to set the Start date to the next work day (excluding weekends), where enddate is the cell reference for the End date of the Predecessor task.</t>
-      </text>
-    </comment>
-    <comment ref="D7" authorId="0">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAC7UcDbU
-Predecessor Tasks    (2019-05-01 20:37:23)
-You can use this column to enter the WBS of a predecessor for reference. The PRO version uses formulas to automatically calculate the Start Date based on the Predecessor.</t>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="0">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAC7UcDbA
-    (2019-05-01 20:37:23)
-Task Lead
-Enter the name of the Task Lead in this column.</t>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAC7UcDa8
-    (2019-05-01 20:37:23)
-Task Description
-Enter the name of each task and sub-task. Use indents for sub-tasks.</t>
+Work Days
+Counts the number of work days, excluding the weekends (Saturday and Sunday). In the PRO version, you can customize the work week and list specific non-working days like holidays. In the PRO version, the default input is the Work Days instead of the Calendar Days.</t>
+        </r>
       </text>
     </comment>
   </commentList>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" roundtripDataSignature="AMtx7mhf77MgxQMm7EEiw9z79VZXI5C+Iw==" r:id="rId1"/>
     </ext>
   </extLst>
@@ -119,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>WBS</t>
   </si>
@@ -246,27 +294,6 @@
     <t>Design</t>
   </si>
   <si>
-    <t>Monitoring and control</t>
-  </si>
-  <si>
-    <t>1.2.1</t>
-  </si>
-  <si>
-    <t>1.2.2</t>
-  </si>
-  <si>
-    <t>1.2.3</t>
-  </si>
-  <si>
-    <t>Peer review</t>
-  </si>
-  <si>
-    <t>Corrective actions</t>
-  </si>
-  <si>
-    <t>Preventive actions</t>
-  </si>
-  <si>
     <t>ITI</t>
   </si>
   <si>
@@ -290,6 +317,12 @@
   <si>
     <t>Maintenance</t>
   </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>HLD</t>
+  </si>
 </sst>
 </file>
 
@@ -301,7 +334,7 @@
     <numFmt numFmtId="166" formatCode="d"/>
     <numFmt numFmtId="167" formatCode="d\ mmm\ yyyy"/>
   </numFmts>
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -461,34 +494,6 @@
       <sz val="11"/>
       <color indexed="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -1066,7 +1071,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -1101,86 +1106,86 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="30" fillId="21" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="26" fillId="21" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="30" fillId="21" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="26" fillId="21" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="30" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="26" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="35" fillId="23" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="31" fillId="23" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="35" fillId="23" borderId="11" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="31" fillId="23" borderId="11" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="35" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="31" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="30" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="30" fillId="21" borderId="13" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="26" fillId="21" borderId="13" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="30" fillId="21" borderId="13" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="26" fillId="21" borderId="13" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="30" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="26" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1189,82 +1194,82 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="39" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="35" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="40" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="36" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="39" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="35" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="39" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="35" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="35" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="26" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="30" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="26" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="26" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1283,123 +1288,117 @@
     <xf numFmtId="9" fontId="15" fillId="19" borderId="10" xfId="29" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="43" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="43" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="31" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="10" xfId="29" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="31" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="31" fillId="22" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="31" fillId="23" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="31" fillId="23" borderId="24" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="26" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="29" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="29" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="15" fillId="19" borderId="0" xfId="29" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="15" fillId="19" borderId="0" xfId="29" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="47" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="47" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="35" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="30" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="10" xfId="29" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="35" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="35" fillId="22" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="35" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="35" fillId="23" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="35" fillId="23" borderId="24" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="30" fillId="21" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="29" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="29" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="19" borderId="0" xfId="29" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="19" borderId="0" xfId="29" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1449,7 +1448,7 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="8">
     <dxf>
       <border>
         <left style="thin">
@@ -1489,46 +1488,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -1561,32 +1520,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1701,7 +1634,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1759,13 +1692,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8238" name="Scroll Bar 46" hidden="1">
+            <xdr:cNvPr id="9262" name="Scroll Bar 46" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s8238"/>
+                  <a14:compatExt spid="_x0000_s9262"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E200000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E200000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1780,11 +1713,24 @@
               <a:avLst/>
             </a:prstGeom>
             <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:noFill/>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData fPrintsWithSheet="0"/>
@@ -1792,6 +1738,49 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1033" name="Rectangle 9" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2085,30 +2074,30 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO55"/>
+  <dimension ref="A1:BO51"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" tabSelected="1" zoomScaleNormal="100">
-      <pane ySplit="7" topLeftCell="A8" state="frozen" activePane="bottomLeft"/>
-      <selection activeCell="E15" pane="bottomLeft" sqref="E15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.88671875" style="5"/>
-    <col customWidth="1" min="2" max="2" width="22.33203125" style="1"/>
-    <col customWidth="1" min="3" max="3" width="10.21875" style="1"/>
-    <col customWidth="1" min="4" hidden="1" max="4" width="6.88671875" style="6"/>
-    <col customWidth="1" min="5" max="5" width="10.21875" style="6"/>
-    <col customWidth="1" min="6" max="7" width="12" style="1"/>
-    <col customWidth="1" min="8" max="8" width="9.33203125" style="1"/>
-    <col customWidth="1" min="9" max="9" width="17.88671875" style="1"/>
-    <col customWidth="1" min="10" max="10" width="6.44140625" style="1"/>
-    <col customWidth="1" min="11" max="11" width="1.88671875" style="1"/>
-    <col customWidth="1" min="12" max="67" width="2.44140625" style="1"/>
+    <col min="1" max="1" width="6.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" style="6" customWidth="1"/>
+    <col min="6" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="1.88671875" style="1" customWidth="1"/>
+    <col min="12" max="67" width="2.44140625" style="1" customWidth="1"/>
     <col min="68" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row spans="1:67" r="1" customHeight="1" x14ac:dyDescent="0.25" ht="30">
+    <row r="1" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="72" t="s">
         <v>11</v>
       </c>
@@ -2119,33 +2108,33 @@
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
       <c r="J1" s="76"/>
-      <c r="L1" s="87" t="s">
+      <c r="L1" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="87"/>
-      <c r="AE1" s="87"/>
-      <c r="AF1" s="87"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="107"/>
+      <c r="X1" s="107"/>
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="107"/>
+      <c r="AB1" s="107"/>
+      <c r="AC1" s="107"/>
+      <c r="AD1" s="107"/>
+      <c r="AE1" s="107"/>
+      <c r="AF1" s="107"/>
     </row>
-    <row spans="1:67" r="2" customHeight="1" x14ac:dyDescent="0.25" ht="18">
+    <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2155,7 +2144,7 @@
       <c r="G2" s="77"/>
       <c r="I2" s="2"/>
     </row>
-    <row spans="1:67" r="3" x14ac:dyDescent="0.25" ht="13.8">
+    <row r="3" spans="1:67" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
       <c r="B3" s="15"/>
       <c r="C3" s="4"/>
@@ -2183,17 +2172,17 @@
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
     </row>
-    <row spans="1:67" r="4" customHeight="1" x14ac:dyDescent="0.25" ht="17.25">
+    <row r="4" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="57"/>
       <c r="B4" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="89">
+      <c r="C4" s="112">
         <v>43582</v>
       </c>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
       <c r="G4" s="58"/>
       <c r="H4" s="61" t="s">
         <v>7</v>
@@ -2203,173 +2192,173 @@
       </c>
       <c r="J4" s="59"/>
       <c r="K4" s="17"/>
-      <c r="L4" s="81" t="str">
+      <c r="L4" s="109" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="81" t="str">
+      <c r="M4" s="110"/>
+      <c r="N4" s="110"/>
+      <c r="O4" s="110"/>
+      <c r="P4" s="110"/>
+      <c r="Q4" s="110"/>
+      <c r="R4" s="111"/>
+      <c r="S4" s="109" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="T4" s="82"/>
-      <c r="U4" s="82"/>
-      <c r="V4" s="82"/>
-      <c r="W4" s="82"/>
-      <c r="X4" s="82"/>
-      <c r="Y4" s="83"/>
-      <c r="Z4" s="81" t="str">
+      <c r="T4" s="110"/>
+      <c r="U4" s="110"/>
+      <c r="V4" s="110"/>
+      <c r="W4" s="110"/>
+      <c r="X4" s="110"/>
+      <c r="Y4" s="111"/>
+      <c r="Z4" s="109" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="AA4" s="82"/>
-      <c r="AB4" s="82"/>
-      <c r="AC4" s="82"/>
-      <c r="AD4" s="82"/>
-      <c r="AE4" s="82"/>
-      <c r="AF4" s="83"/>
-      <c r="AG4" s="81" t="str">
+      <c r="AA4" s="110"/>
+      <c r="AB4" s="110"/>
+      <c r="AC4" s="110"/>
+      <c r="AD4" s="110"/>
+      <c r="AE4" s="110"/>
+      <c r="AF4" s="111"/>
+      <c r="AG4" s="109" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AH4" s="82"/>
-      <c r="AI4" s="82"/>
-      <c r="AJ4" s="82"/>
-      <c r="AK4" s="82"/>
-      <c r="AL4" s="82"/>
-      <c r="AM4" s="83"/>
-      <c r="AN4" s="81" t="str">
+      <c r="AH4" s="110"/>
+      <c r="AI4" s="110"/>
+      <c r="AJ4" s="110"/>
+      <c r="AK4" s="110"/>
+      <c r="AL4" s="110"/>
+      <c r="AM4" s="111"/>
+      <c r="AN4" s="109" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AO4" s="82"/>
-      <c r="AP4" s="82"/>
-      <c r="AQ4" s="82"/>
-      <c r="AR4" s="82"/>
-      <c r="AS4" s="82"/>
-      <c r="AT4" s="83"/>
-      <c r="AU4" s="81" t="str">
+      <c r="AO4" s="110"/>
+      <c r="AP4" s="110"/>
+      <c r="AQ4" s="110"/>
+      <c r="AR4" s="110"/>
+      <c r="AS4" s="110"/>
+      <c r="AT4" s="111"/>
+      <c r="AU4" s="109" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AV4" s="82"/>
-      <c r="AW4" s="82"/>
-      <c r="AX4" s="82"/>
-      <c r="AY4" s="82"/>
-      <c r="AZ4" s="82"/>
-      <c r="BA4" s="92"/>
-      <c r="BB4" s="91"/>
-      <c r="BC4" s="91"/>
-      <c r="BD4" s="91"/>
-      <c r="BE4" s="91"/>
-      <c r="BF4" s="91"/>
-      <c r="BG4" s="91"/>
-      <c r="BH4" s="91"/>
-      <c r="BI4" s="91"/>
-      <c r="BJ4" s="91"/>
-      <c r="BK4" s="91"/>
-      <c r="BL4" s="91"/>
-      <c r="BM4" s="91"/>
-      <c r="BN4" s="91"/>
-      <c r="BO4" s="91"/>
+      <c r="AV4" s="110"/>
+      <c r="AW4" s="110"/>
+      <c r="AX4" s="110"/>
+      <c r="AY4" s="110"/>
+      <c r="AZ4" s="110"/>
+      <c r="BA4" s="116"/>
+      <c r="BB4" s="106"/>
+      <c r="BC4" s="106"/>
+      <c r="BD4" s="106"/>
+      <c r="BE4" s="106"/>
+      <c r="BF4" s="106"/>
+      <c r="BG4" s="106"/>
+      <c r="BH4" s="106"/>
+      <c r="BI4" s="106"/>
+      <c r="BJ4" s="106"/>
+      <c r="BK4" s="106"/>
+      <c r="BL4" s="106"/>
+      <c r="BM4" s="106"/>
+      <c r="BN4" s="106"/>
+      <c r="BO4" s="106"/>
     </row>
-    <row spans="1:67" r="5" customHeight="1" x14ac:dyDescent="0.25" ht="17.25">
+    <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57"/>
       <c r="B5" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
       <c r="G5" s="60"/>
       <c r="H5" s="60"/>
       <c r="I5" s="60"/>
       <c r="J5" s="60"/>
       <c r="K5" s="17"/>
-      <c r="L5" s="84">
+      <c r="L5" s="113">
         <f>L6</f>
         <v>43577</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="114"/>
+      <c r="N5" s="114"/>
+      <c r="O5" s="114"/>
+      <c r="P5" s="114"/>
+      <c r="Q5" s="114"/>
+      <c r="R5" s="115"/>
+      <c r="S5" s="113">
         <f>S6</f>
         <v>43584</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="114"/>
+      <c r="U5" s="114"/>
+      <c r="V5" s="114"/>
+      <c r="W5" s="114"/>
+      <c r="X5" s="114"/>
+      <c r="Y5" s="115"/>
+      <c r="Z5" s="113">
         <f>Z6</f>
         <v>43591</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="114"/>
+      <c r="AB5" s="114"/>
+      <c r="AC5" s="114"/>
+      <c r="AD5" s="114"/>
+      <c r="AE5" s="114"/>
+      <c r="AF5" s="115"/>
+      <c r="AG5" s="113">
         <f>AG6</f>
         <v>43598</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="114"/>
+      <c r="AI5" s="114"/>
+      <c r="AJ5" s="114"/>
+      <c r="AK5" s="114"/>
+      <c r="AL5" s="114"/>
+      <c r="AM5" s="115"/>
+      <c r="AN5" s="113">
         <f>AN6</f>
         <v>43605</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="114"/>
+      <c r="AP5" s="114"/>
+      <c r="AQ5" s="114"/>
+      <c r="AR5" s="114"/>
+      <c r="AS5" s="114"/>
+      <c r="AT5" s="115"/>
+      <c r="AU5" s="113">
         <f>AU6</f>
         <v>43612</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="93"/>
-      <c r="BB5" s="90"/>
-      <c r="BC5" s="90"/>
-      <c r="BD5" s="90"/>
-      <c r="BE5" s="90"/>
-      <c r="BF5" s="90"/>
-      <c r="BG5" s="90"/>
-      <c r="BH5" s="90"/>
-      <c r="BI5" s="90"/>
-      <c r="BJ5" s="90"/>
-      <c r="BK5" s="90"/>
-      <c r="BL5" s="90"/>
-      <c r="BM5" s="90"/>
-      <c r="BN5" s="90"/>
-      <c r="BO5" s="90"/>
+      <c r="AV5" s="114"/>
+      <c r="AW5" s="114"/>
+      <c r="AX5" s="114"/>
+      <c r="AY5" s="114"/>
+      <c r="AZ5" s="114"/>
+      <c r="BA5" s="117"/>
+      <c r="BB5" s="105"/>
+      <c r="BC5" s="105"/>
+      <c r="BD5" s="105"/>
+      <c r="BE5" s="105"/>
+      <c r="BF5" s="105"/>
+      <c r="BG5" s="105"/>
+      <c r="BH5" s="105"/>
+      <c r="BI5" s="105"/>
+      <c r="BJ5" s="105"/>
+      <c r="BK5" s="105"/>
+      <c r="BL5" s="105"/>
+      <c r="BM5" s="105"/>
+      <c r="BN5" s="105"/>
+      <c r="BO5" s="105"/>
     </row>
-    <row spans="1:67" r="6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -2386,7 +2375,7 @@
         <v>43577</v>
       </c>
       <c r="M6" s="37">
-        <f ref="M6:AR6" t="shared" si="0">L6+1</f>
+        <f t="shared" ref="M6:AR6" si="0">L6+1</f>
         <v>43578</v>
       </c>
       <c r="N6" s="37">
@@ -2514,7 +2503,7 @@
         <v>43609</v>
       </c>
       <c r="AS6" s="37">
-        <f ref="AS6:BA6" t="shared" si="1">AR6+1</f>
+        <f t="shared" ref="AS6:BA6" si="1">AR6+1</f>
         <v>43610</v>
       </c>
       <c r="AT6" s="46">
@@ -2545,26 +2534,26 @@
         <f t="shared" si="1"/>
         <v>43617</v>
       </c>
-      <c r="BA6" s="94">
+      <c r="BA6" s="81">
         <f t="shared" si="1"/>
         <v>43618</v>
       </c>
-      <c r="BB6" s="96"/>
-      <c r="BC6" s="96"/>
-      <c r="BD6" s="96"/>
-      <c r="BE6" s="96"/>
-      <c r="BF6" s="96"/>
-      <c r="BG6" s="96"/>
-      <c r="BH6" s="96"/>
-      <c r="BI6" s="96"/>
-      <c r="BJ6" s="96"/>
-      <c r="BK6" s="96"/>
-      <c r="BL6" s="96"/>
-      <c r="BM6" s="96"/>
-      <c r="BN6" s="96"/>
-      <c r="BO6" s="96"/>
+      <c r="BB6" s="83"/>
+      <c r="BC6" s="83"/>
+      <c r="BD6" s="83"/>
+      <c r="BE6" s="83"/>
+      <c r="BF6" s="83"/>
+      <c r="BG6" s="83"/>
+      <c r="BH6" s="83"/>
+      <c r="BI6" s="83"/>
+      <c r="BJ6" s="83"/>
+      <c r="BK6" s="83"/>
+      <c r="BL6" s="83"/>
+      <c r="BM6" s="83"/>
+      <c r="BN6" s="83"/>
+      <c r="BO6" s="83"/>
     </row>
-    <row spans="1:67" r="7" s="71" thickBot="1" x14ac:dyDescent="0.3" ht="24.6" customFormat="1">
+    <row r="7" spans="1:67" s="71" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="63" t="s">
         <v>0</v>
       </c>
@@ -2578,7 +2567,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="66" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F7" s="67" t="s">
         <v>2</v>
@@ -2597,7 +2586,7 @@
       </c>
       <c r="K7" s="65"/>
       <c r="L7" s="68" t="str">
-        <f ref="L7:AQ7" t="shared" si="2">CHOOSE(WEEKDAY(L6,1),"S","M","T","W","T","F","S")</f>
+        <f t="shared" ref="L7:AQ7" si="2">CHOOSE(WEEKDAY(L6,1),"S","M","T","W","T","F","S")</f>
         <v>M</v>
       </c>
       <c r="M7" s="69" t="str">
@@ -2725,7 +2714,7 @@
         <v>T</v>
       </c>
       <c r="AR7" s="69" t="str">
-        <f ref="AR7:BA7" t="shared" si="3">CHOOSE(WEEKDAY(AR6,1),"S","M","T","W","T","F","S")</f>
+        <f t="shared" ref="AR7:BA7" si="3">CHOOSE(WEEKDAY(AR6,1),"S","M","T","W","T","F","S")</f>
         <v>F</v>
       </c>
       <c r="AS7" s="69" t="str">
@@ -2760,26 +2749,26 @@
         <f t="shared" si="3"/>
         <v>S</v>
       </c>
-      <c r="BA7" s="95" t="str">
+      <c r="BA7" s="82" t="str">
         <f t="shared" si="3"/>
         <v>S</v>
       </c>
-      <c r="BB7" s="97"/>
-      <c r="BC7" s="97"/>
-      <c r="BD7" s="97"/>
-      <c r="BE7" s="97"/>
-      <c r="BF7" s="97"/>
-      <c r="BG7" s="97"/>
-      <c r="BH7" s="97"/>
-      <c r="BI7" s="97"/>
-      <c r="BJ7" s="97"/>
-      <c r="BK7" s="97"/>
-      <c r="BL7" s="97"/>
-      <c r="BM7" s="97"/>
-      <c r="BN7" s="97"/>
-      <c r="BO7" s="97"/>
+      <c r="BB7" s="84"/>
+      <c r="BC7" s="84"/>
+      <c r="BD7" s="84"/>
+      <c r="BE7" s="84"/>
+      <c r="BF7" s="84"/>
+      <c r="BG7" s="84"/>
+      <c r="BH7" s="84"/>
+      <c r="BI7" s="84"/>
+      <c r="BJ7" s="84"/>
+      <c r="BK7" s="84"/>
+      <c r="BL7" s="84"/>
+      <c r="BM7" s="84"/>
+      <c r="BN7" s="84"/>
+      <c r="BO7" s="84"/>
     </row>
-    <row spans="1:67" r="8" s="22" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="8" spans="1:67" s="22" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="38"/>
       <c r="B8" s="39" t="s">
         <v>32</v>
@@ -2787,16 +2776,16 @@
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
-      <c r="F8" s="106">
+      <c r="F8" s="91">
         <v>43582</v>
       </c>
-      <c r="G8" s="105">
+      <c r="G8" s="90">
         <v>43589</v>
       </c>
       <c r="H8" s="42"/>
       <c r="I8" s="43"/>
       <c r="J8" s="44">
-        <f ref="J8:J48" t="shared" si="4">IF(OR(G8=0,F8=0)," - ",NETWORKDAYS(F8,G8))</f>
+        <f t="shared" ref="J8:J44" si="4">IF(OR(G8=0,F8=0)," - ",NETWORKDAYS(F8,G8))</f>
         <v>5</v>
       </c>
       <c r="K8" s="47"/>
@@ -2857,29 +2846,29 @@
       <c r="BN8" s="53"/>
       <c r="BO8" s="53"/>
     </row>
-    <row spans="1:67" r="9" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A9" s="100">
+    <row r="9" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A9" s="86">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="103" t="s">
+      <c r="C9" s="89" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="74"/>
       <c r="E9" s="74"/>
-      <c r="F9" s="107">
+      <c r="F9" s="92">
         <v>43582</v>
       </c>
-      <c r="G9" s="110">
-        <v>43615</v>
+      <c r="G9" s="95">
+        <v>43589</v>
       </c>
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
       <c r="J9" s="31">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="K9" s="48"/>
       <c r="L9" s="54"/>
@@ -2939,33 +2928,33 @@
       <c r="BN9" s="54"/>
       <c r="BO9" s="54"/>
     </row>
-    <row spans="1:67" r="10" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="10" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="102" t="s">
+      <c r="B10" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="103" t="s">
+      <c r="C10" s="89" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="74"/>
       <c r="E10" s="74"/>
-      <c r="F10" s="107">
+      <c r="F10" s="92">
         <v>43582</v>
       </c>
-      <c r="G10" s="110">
-        <v>43615</v>
+      <c r="G10" s="95">
+        <v>43587</v>
       </c>
       <c r="H10" s="29">
         <v>2</v>
       </c>
       <c r="I10" s="30">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
       <c r="J10" s="31">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="K10" s="48"/>
       <c r="L10" s="54"/>
@@ -3025,25 +3014,29 @@
       <c r="BN10" s="54"/>
       <c r="BO10" s="54"/>
     </row>
-    <row spans="1:67" r="11" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="11" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="102" t="s">
+      <c r="B11" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="89" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="74"/>
       <c r="E11" s="74"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="110"/>
+      <c r="F11" s="92">
+        <v>43583</v>
+      </c>
+      <c r="G11" s="95">
+        <v>43588</v>
+      </c>
       <c r="H11" s="29"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="31" t="str">
+      <c r="J11" s="31">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
+        <v>5</v>
       </c>
       <c r="K11" s="48"/>
       <c r="L11" s="54"/>
@@ -3103,22 +3096,22 @@
       <c r="BN11" s="54"/>
       <c r="BO11" s="54"/>
     </row>
-    <row spans="1:67" r="12" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="12" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="102" t="s">
+      <c r="B12" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="103" t="s">
+      <c r="C12" s="89" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="74"/>
       <c r="E12" s="74"/>
-      <c r="F12" s="107">
+      <c r="F12" s="92">
         <v>43583</v>
       </c>
-      <c r="G12" s="110">
+      <c r="G12" s="95">
         <v>43586</v>
       </c>
       <c r="H12" s="29"/>
@@ -3187,25 +3180,25 @@
       <c r="BN12" s="54"/>
       <c r="BO12" s="54"/>
     </row>
-    <row spans="1:67" r="13" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="13" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.4</v>
       </c>
-      <c r="B13" s="102" t="s">
+      <c r="B13" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="89" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="74"/>
       <c r="E13" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="107">
+      <c r="F13" s="92">
         <v>43583</v>
       </c>
-      <c r="G13" s="110">
+      <c r="G13" s="95">
         <v>43586</v>
       </c>
       <c r="H13" s="29"/>
@@ -3274,28 +3267,28 @@
       <c r="BN13" s="54"/>
       <c r="BO13" s="54"/>
     </row>
-    <row spans="1:67" r="14" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="14" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.5</v>
       </c>
-      <c r="B14" s="102" t="s">
+      <c r="B14" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="89" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="74"/>
       <c r="E14" s="74"/>
-      <c r="F14" s="107">
+      <c r="F14" s="92">
         <v>43583</v>
       </c>
-      <c r="G14" s="110">
+      <c r="G14" s="95">
         <v>43587</v>
       </c>
       <c r="H14" s="29"/>
       <c r="I14" s="30">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J14" s="31">
         <f t="shared" si="4"/>
@@ -3359,23 +3352,23 @@
       <c r="BN14" s="54"/>
       <c r="BO14" s="54"/>
     </row>
-    <row spans="1:67" r="15" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="15" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.6</v>
       </c>
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="103" t="s">
+      <c r="C15" s="89" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="74"/>
       <c r="E15" s="74"/>
-      <c r="F15" s="107">
+      <c r="F15" s="92">
         <v>43583</v>
       </c>
-      <c r="G15" s="110">
+      <c r="G15" s="95">
         <v>43583</v>
       </c>
       <c r="H15" s="29"/>
@@ -3444,30 +3437,30 @@
       <c r="BN15" s="54"/>
       <c r="BO15" s="54"/>
     </row>
-    <row spans="1:67" r="16" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="16" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.7</v>
       </c>
-      <c r="B16" s="102" t="s">
+      <c r="B16" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="103" t="s">
+      <c r="C16" s="89" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="74"/>
       <c r="E16" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="107">
+      <c r="F16" s="92">
         <v>43585</v>
       </c>
-      <c r="G16" s="110">
+      <c r="G16" s="95">
         <v>43610</v>
       </c>
       <c r="H16" s="29"/>
       <c r="I16" s="30">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
       <c r="J16" s="31">
         <f t="shared" si="4"/>
@@ -3531,103 +3524,101 @@
       <c r="BN16" s="54"/>
       <c r="BO16" s="54"/>
     </row>
-    <row spans="1:67" r="17" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A17" s="100">
-        <v>1.2</v>
-      </c>
-      <c r="B17" s="98" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="103"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="107"/>
-      <c r="G17" s="110"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="30">
-        <v>0</v>
-      </c>
-      <c r="J17" s="31" t="str">
+    <row r="17" spans="1:67" s="22" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="26" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K17" s="48"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="54"/>
-      <c r="T17" s="54"/>
-      <c r="U17" s="54"/>
-      <c r="V17" s="54"/>
-      <c r="W17" s="54"/>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="54"/>
-      <c r="Z17" s="54"/>
-      <c r="AA17" s="54"/>
-      <c r="AB17" s="54"/>
-      <c r="AC17" s="54"/>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="54"/>
-      <c r="AF17" s="54"/>
-      <c r="AG17" s="54"/>
-      <c r="AH17" s="54"/>
-      <c r="AI17" s="54"/>
-      <c r="AJ17" s="54"/>
-      <c r="AK17" s="54"/>
-      <c r="AL17" s="54"/>
-      <c r="AM17" s="54"/>
-      <c r="AN17" s="54"/>
-      <c r="AO17" s="54"/>
-      <c r="AP17" s="54"/>
-      <c r="AQ17" s="54"/>
-      <c r="AR17" s="54"/>
-      <c r="AS17" s="54"/>
-      <c r="AT17" s="54"/>
-      <c r="AU17" s="54"/>
-      <c r="AV17" s="54"/>
-      <c r="AW17" s="54"/>
-      <c r="AX17" s="54"/>
-      <c r="AY17" s="54"/>
-      <c r="AZ17" s="54"/>
-      <c r="BA17" s="54"/>
-      <c r="BB17" s="54"/>
-      <c r="BC17" s="54"/>
-      <c r="BD17" s="54"/>
-      <c r="BE17" s="54"/>
-      <c r="BF17" s="54"/>
-      <c r="BG17" s="54"/>
-      <c r="BH17" s="54"/>
-      <c r="BI17" s="54"/>
-      <c r="BJ17" s="54"/>
-      <c r="BK17" s="54"/>
-      <c r="BL17" s="54"/>
-      <c r="BM17" s="54"/>
-      <c r="BN17" s="54"/>
-      <c r="BO17" s="54"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="56"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
+      <c r="Y17" s="56"/>
+      <c r="Z17" s="56"/>
+      <c r="AA17" s="56"/>
+      <c r="AB17" s="56"/>
+      <c r="AC17" s="56"/>
+      <c r="AD17" s="56"/>
+      <c r="AE17" s="56"/>
+      <c r="AF17" s="56"/>
+      <c r="AG17" s="56"/>
+      <c r="AH17" s="56"/>
+      <c r="AI17" s="56"/>
+      <c r="AJ17" s="56"/>
+      <c r="AK17" s="56"/>
+      <c r="AL17" s="56"/>
+      <c r="AM17" s="56"/>
+      <c r="AN17" s="56"/>
+      <c r="AO17" s="56"/>
+      <c r="AP17" s="56"/>
+      <c r="AQ17" s="56"/>
+      <c r="AR17" s="56"/>
+      <c r="AS17" s="56"/>
+      <c r="AT17" s="56"/>
+      <c r="AU17" s="56"/>
+      <c r="AV17" s="56"/>
+      <c r="AW17" s="56"/>
+      <c r="AX17" s="56"/>
+      <c r="AY17" s="56"/>
+      <c r="AZ17" s="56"/>
+      <c r="BA17" s="56"/>
+      <c r="BB17" s="56"/>
+      <c r="BC17" s="56"/>
+      <c r="BD17" s="56"/>
+      <c r="BE17" s="56"/>
+      <c r="BF17" s="56"/>
+      <c r="BG17" s="56"/>
+      <c r="BH17" s="56"/>
+      <c r="BI17" s="56"/>
+      <c r="BJ17" s="56"/>
+      <c r="BK17" s="56"/>
+      <c r="BL17" s="56"/>
+      <c r="BM17" s="56"/>
+      <c r="BN17" s="56"/>
+      <c r="BO17" s="56"/>
     </row>
-    <row spans="1:67" r="18" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A18" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="102" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="104"/>
+    <row r="18" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A18" s="27">
+        <v>2.1</v>
+      </c>
+      <c r="B18" s="87" t="s">
+        <v>34</v>
+      </c>
       <c r="D18" s="74"/>
       <c r="E18" s="74"/>
-      <c r="F18" s="107"/>
-      <c r="G18"/>
+      <c r="F18" s="92">
+        <v>43589</v>
+      </c>
+      <c r="G18" s="51">
+        <v>43596</v>
+      </c>
       <c r="H18" s="29"/>
       <c r="I18" s="30">
         <v>0</v>
       </c>
-      <c r="J18" s="31" t="str">
+      <c r="J18" s="31">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
+        <v>5</v>
       </c>
       <c r="K18" s="48"/>
       <c r="L18" s="54"/>
@@ -3687,23 +3678,25 @@
       <c r="BN18" s="54"/>
       <c r="BO18" s="54"/>
     </row>
-    <row spans="1:67" r="19" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="19" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="102" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="103" t="s">
-        <v>22</v>
+        <v>43</v>
+      </c>
+      <c r="B19" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="D19" s="74"/>
       <c r="E19" s="74"/>
-      <c r="F19" s="107"/>
-      <c r="G19"/>
+      <c r="F19" s="92">
+        <v>43590</v>
+      </c>
+      <c r="G19" s="51"/>
       <c r="H19" s="29"/>
       <c r="I19" s="30">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J19" s="31" t="str">
         <f t="shared" si="4"/>
@@ -3767,17 +3760,13 @@
       <c r="BN19" s="54"/>
       <c r="BO19" s="54"/>
     </row>
-    <row spans="1:67" r="20" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A20" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="102" t="s">
-        <v>41</v>
-      </c>
+    <row r="20" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="73"/>
       <c r="D20" s="74"/>
       <c r="E20" s="74"/>
-      <c r="F20" s="107"/>
-      <c r="G20"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="51"/>
       <c r="H20" s="29"/>
       <c r="I20" s="30">
         <v>0</v>
@@ -3844,101 +3833,93 @@
       <c r="BN20" s="54"/>
       <c r="BO20" s="54"/>
     </row>
-    <row spans="1:67" r="21" s="22" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="108"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="26" t="str">
+    <row r="21" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="73"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="92"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="30">
+        <v>0</v>
+      </c>
+      <c r="J21" s="31" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K21" s="49"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
-      <c r="S21" s="56"/>
-      <c r="T21" s="56"/>
-      <c r="U21" s="56"/>
-      <c r="V21" s="56"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="56"/>
-      <c r="Y21" s="56"/>
-      <c r="Z21" s="56"/>
-      <c r="AA21" s="56"/>
-      <c r="AB21" s="56"/>
-      <c r="AC21" s="56"/>
-      <c r="AD21" s="56"/>
-      <c r="AE21" s="56"/>
-      <c r="AF21" s="56"/>
-      <c r="AG21" s="56"/>
-      <c r="AH21" s="56"/>
-      <c r="AI21" s="56"/>
-      <c r="AJ21" s="56"/>
-      <c r="AK21" s="56"/>
-      <c r="AL21" s="56"/>
-      <c r="AM21" s="56"/>
-      <c r="AN21" s="56"/>
-      <c r="AO21" s="56"/>
-      <c r="AP21" s="56"/>
-      <c r="AQ21" s="56"/>
-      <c r="AR21" s="56"/>
-      <c r="AS21" s="56"/>
-      <c r="AT21" s="56"/>
-      <c r="AU21" s="56"/>
-      <c r="AV21" s="56"/>
-      <c r="AW21" s="56"/>
-      <c r="AX21" s="56"/>
-      <c r="AY21" s="56"/>
-      <c r="AZ21" s="56"/>
-      <c r="BA21" s="56"/>
-      <c r="BB21" s="56"/>
-      <c r="BC21" s="56"/>
-      <c r="BD21" s="56"/>
-      <c r="BE21" s="56"/>
-      <c r="BF21" s="56"/>
-      <c r="BG21" s="56"/>
-      <c r="BH21" s="56"/>
-      <c r="BI21" s="56"/>
-      <c r="BJ21" s="56"/>
-      <c r="BK21" s="56"/>
-      <c r="BL21" s="56"/>
-      <c r="BM21" s="56"/>
-      <c r="BN21" s="56"/>
-      <c r="BO21" s="56"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="54"/>
+      <c r="T21" s="54"/>
+      <c r="U21" s="54"/>
+      <c r="V21" s="54"/>
+      <c r="W21" s="54"/>
+      <c r="X21" s="54"/>
+      <c r="Y21" s="54"/>
+      <c r="Z21" s="54"/>
+      <c r="AA21" s="54"/>
+      <c r="AB21" s="54"/>
+      <c r="AC21" s="54"/>
+      <c r="AD21" s="54"/>
+      <c r="AE21" s="54"/>
+      <c r="AF21" s="54"/>
+      <c r="AG21" s="54"/>
+      <c r="AH21" s="54"/>
+      <c r="AI21" s="54"/>
+      <c r="AJ21" s="54"/>
+      <c r="AK21" s="54"/>
+      <c r="AL21" s="54"/>
+      <c r="AM21" s="54"/>
+      <c r="AN21" s="54"/>
+      <c r="AO21" s="54"/>
+      <c r="AP21" s="54"/>
+      <c r="AQ21" s="54"/>
+      <c r="AR21" s="54"/>
+      <c r="AS21" s="54"/>
+      <c r="AT21" s="54"/>
+      <c r="AU21" s="54"/>
+      <c r="AV21" s="54"/>
+      <c r="AW21" s="54"/>
+      <c r="AX21" s="54"/>
+      <c r="AY21" s="54"/>
+      <c r="AZ21" s="54"/>
+      <c r="BA21" s="54"/>
+      <c r="BB21" s="54"/>
+      <c r="BC21" s="54"/>
+      <c r="BD21" s="54"/>
+      <c r="BE21" s="54"/>
+      <c r="BF21" s="54"/>
+      <c r="BG21" s="54"/>
+      <c r="BH21" s="54"/>
+      <c r="BI21" s="54"/>
+      <c r="BJ21" s="54"/>
+      <c r="BK21" s="54"/>
+      <c r="BL21" s="54"/>
+      <c r="BM21" s="54"/>
+      <c r="BN21" s="54"/>
+      <c r="BO21" s="54"/>
     </row>
-    <row spans="1:67" r="22" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A22" s="27">
-        <v>2.1</v>
-      </c>
-      <c r="B22" s="101" t="s">
-        <v>34</v>
-      </c>
+    <row r="22" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="73"/>
       <c r="D22" s="74"/>
       <c r="E22" s="74"/>
-      <c r="F22" s="107">
-        <v>43589</v>
-      </c>
-      <c r="G22" s="51">
-        <v>43596</v>
-      </c>
+      <c r="F22" s="92"/>
+      <c r="G22" s="51"/>
       <c r="H22" s="29"/>
       <c r="I22" s="30">
         <v>0</v>
       </c>
-      <c r="J22" s="31">
+      <c r="J22" s="31" t="str">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v xml:space="preserve"> - </v>
       </c>
       <c r="K22" s="48"/>
       <c r="L22" s="54"/>
@@ -3998,85 +3979,89 @@
       <c r="BN22" s="54"/>
       <c r="BO22" s="54"/>
     </row>
-    <row spans="1:67" r="23" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A23" s="27"/>
-      <c r="B23" s="73"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="107"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="30">
-        <v>0</v>
-      </c>
-      <c r="J23" s="31" t="str">
+    <row r="23" spans="1:67" s="22" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="26" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K23" s="48"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="54"/>
-      <c r="T23" s="54"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="54"/>
-      <c r="W23" s="54"/>
-      <c r="X23" s="54"/>
-      <c r="Y23" s="54"/>
-      <c r="Z23" s="54"/>
-      <c r="AA23" s="54"/>
-      <c r="AB23" s="54"/>
-      <c r="AC23" s="54"/>
-      <c r="AD23" s="54"/>
-      <c r="AE23" s="54"/>
-      <c r="AF23" s="54"/>
-      <c r="AG23" s="54"/>
-      <c r="AH23" s="54"/>
-      <c r="AI23" s="54"/>
-      <c r="AJ23" s="54"/>
-      <c r="AK23" s="54"/>
-      <c r="AL23" s="54"/>
-      <c r="AM23" s="54"/>
-      <c r="AN23" s="54"/>
-      <c r="AO23" s="54"/>
-      <c r="AP23" s="54"/>
-      <c r="AQ23" s="54"/>
-      <c r="AR23" s="54"/>
-      <c r="AS23" s="54"/>
-      <c r="AT23" s="54"/>
-      <c r="AU23" s="54"/>
-      <c r="AV23" s="54"/>
-      <c r="AW23" s="54"/>
-      <c r="AX23" s="54"/>
-      <c r="AY23" s="54"/>
-      <c r="AZ23" s="54"/>
-      <c r="BA23" s="54"/>
-      <c r="BB23" s="54"/>
-      <c r="BC23" s="54"/>
-      <c r="BD23" s="54"/>
-      <c r="BE23" s="54"/>
-      <c r="BF23" s="54"/>
-      <c r="BG23" s="54"/>
-      <c r="BH23" s="54"/>
-      <c r="BI23" s="54"/>
-      <c r="BJ23" s="54"/>
-      <c r="BK23" s="54"/>
-      <c r="BL23" s="54"/>
-      <c r="BM23" s="54"/>
-      <c r="BN23" s="54"/>
-      <c r="BO23" s="54"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="56"/>
+      <c r="R23" s="56"/>
+      <c r="S23" s="56"/>
+      <c r="T23" s="56"/>
+      <c r="U23" s="56"/>
+      <c r="V23" s="56"/>
+      <c r="W23" s="56"/>
+      <c r="X23" s="56"/>
+      <c r="Y23" s="56"/>
+      <c r="Z23" s="56"/>
+      <c r="AA23" s="56"/>
+      <c r="AB23" s="56"/>
+      <c r="AC23" s="56"/>
+      <c r="AD23" s="56"/>
+      <c r="AE23" s="56"/>
+      <c r="AF23" s="56"/>
+      <c r="AG23" s="56"/>
+      <c r="AH23" s="56"/>
+      <c r="AI23" s="56"/>
+      <c r="AJ23" s="56"/>
+      <c r="AK23" s="56"/>
+      <c r="AL23" s="56"/>
+      <c r="AM23" s="56"/>
+      <c r="AN23" s="56"/>
+      <c r="AO23" s="56"/>
+      <c r="AP23" s="56"/>
+      <c r="AQ23" s="56"/>
+      <c r="AR23" s="56"/>
+      <c r="AS23" s="56"/>
+      <c r="AT23" s="56"/>
+      <c r="AU23" s="56"/>
+      <c r="AV23" s="56"/>
+      <c r="AW23" s="56"/>
+      <c r="AX23" s="56"/>
+      <c r="AY23" s="56"/>
+      <c r="AZ23" s="56"/>
+      <c r="BA23" s="56"/>
+      <c r="BB23" s="56"/>
+      <c r="BC23" s="56"/>
+      <c r="BD23" s="56"/>
+      <c r="BE23" s="56"/>
+      <c r="BF23" s="56"/>
+      <c r="BG23" s="56"/>
+      <c r="BH23" s="56"/>
+      <c r="BI23" s="56"/>
+      <c r="BJ23" s="56"/>
+      <c r="BK23" s="56"/>
+      <c r="BL23" s="56"/>
+      <c r="BM23" s="56"/>
+      <c r="BN23" s="56"/>
+      <c r="BO23" s="56"/>
     </row>
-    <row spans="1:67" r="24" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A24" s="27"/>
-      <c r="B24" s="73"/>
+    <row r="24" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A24" s="27">
+        <v>3.1</v>
+      </c>
+      <c r="B24" s="73" t="s">
+        <v>38</v>
+      </c>
       <c r="D24" s="74"/>
       <c r="E24" s="74"/>
-      <c r="F24" s="107"/>
+      <c r="F24" s="92"/>
       <c r="G24" s="51"/>
       <c r="H24" s="29"/>
       <c r="I24" s="30">
@@ -4144,12 +4129,12 @@
       <c r="BN24" s="54"/>
       <c r="BO24" s="54"/>
     </row>
-    <row spans="1:67" r="25" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="25" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
       <c r="B25" s="73"/>
       <c r="D25" s="74"/>
       <c r="E25" s="74"/>
-      <c r="F25" s="107"/>
+      <c r="F25" s="92"/>
       <c r="G25" s="51"/>
       <c r="H25" s="29"/>
       <c r="I25" s="30">
@@ -4217,12 +4202,12 @@
       <c r="BN25" s="54"/>
       <c r="BO25" s="54"/>
     </row>
-    <row spans="1:67" r="26" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="26" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="73"/>
       <c r="D26" s="74"/>
       <c r="E26" s="74"/>
-      <c r="F26" s="107"/>
+      <c r="F26" s="92"/>
       <c r="G26" s="51"/>
       <c r="H26" s="29"/>
       <c r="I26" s="30">
@@ -4290,89 +4275,85 @@
       <c r="BN26" s="54"/>
       <c r="BO26" s="54"/>
     </row>
-    <row spans="1:67" r="27" s="22" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A27" s="20"/>
-      <c r="B27" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="108"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="26" t="str">
+    <row r="27" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A27" s="27"/>
+      <c r="B27" s="73"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="92"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="30">
+        <v>0</v>
+      </c>
+      <c r="J27" s="31" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K27" s="49"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="56"/>
-      <c r="O27" s="56"/>
-      <c r="P27" s="56"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="56"/>
-      <c r="S27" s="56"/>
-      <c r="T27" s="56"/>
-      <c r="U27" s="56"/>
-      <c r="V27" s="56"/>
-      <c r="W27" s="56"/>
-      <c r="X27" s="56"/>
-      <c r="Y27" s="56"/>
-      <c r="Z27" s="56"/>
-      <c r="AA27" s="56"/>
-      <c r="AB27" s="56"/>
-      <c r="AC27" s="56"/>
-      <c r="AD27" s="56"/>
-      <c r="AE27" s="56"/>
-      <c r="AF27" s="56"/>
-      <c r="AG27" s="56"/>
-      <c r="AH27" s="56"/>
-      <c r="AI27" s="56"/>
-      <c r="AJ27" s="56"/>
-      <c r="AK27" s="56"/>
-      <c r="AL27" s="56"/>
-      <c r="AM27" s="56"/>
-      <c r="AN27" s="56"/>
-      <c r="AO27" s="56"/>
-      <c r="AP27" s="56"/>
-      <c r="AQ27" s="56"/>
-      <c r="AR27" s="56"/>
-      <c r="AS27" s="56"/>
-      <c r="AT27" s="56"/>
-      <c r="AU27" s="56"/>
-      <c r="AV27" s="56"/>
-      <c r="AW27" s="56"/>
-      <c r="AX27" s="56"/>
-      <c r="AY27" s="56"/>
-      <c r="AZ27" s="56"/>
-      <c r="BA27" s="56"/>
-      <c r="BB27" s="56"/>
-      <c r="BC27" s="56"/>
-      <c r="BD27" s="56"/>
-      <c r="BE27" s="56"/>
-      <c r="BF27" s="56"/>
-      <c r="BG27" s="56"/>
-      <c r="BH27" s="56"/>
-      <c r="BI27" s="56"/>
-      <c r="BJ27" s="56"/>
-      <c r="BK27" s="56"/>
-      <c r="BL27" s="56"/>
-      <c r="BM27" s="56"/>
-      <c r="BN27" s="56"/>
-      <c r="BO27" s="56"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="54"/>
+      <c r="P27" s="54"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="54"/>
+      <c r="S27" s="54"/>
+      <c r="T27" s="54"/>
+      <c r="U27" s="54"/>
+      <c r="V27" s="54"/>
+      <c r="W27" s="54"/>
+      <c r="X27" s="54"/>
+      <c r="Y27" s="54"/>
+      <c r="Z27" s="54"/>
+      <c r="AA27" s="54"/>
+      <c r="AB27" s="54"/>
+      <c r="AC27" s="54"/>
+      <c r="AD27" s="54"/>
+      <c r="AE27" s="54"/>
+      <c r="AF27" s="54"/>
+      <c r="AG27" s="54"/>
+      <c r="AH27" s="54"/>
+      <c r="AI27" s="54"/>
+      <c r="AJ27" s="54"/>
+      <c r="AK27" s="54"/>
+      <c r="AL27" s="54"/>
+      <c r="AM27" s="54"/>
+      <c r="AN27" s="54"/>
+      <c r="AO27" s="54"/>
+      <c r="AP27" s="54"/>
+      <c r="AQ27" s="54"/>
+      <c r="AR27" s="54"/>
+      <c r="AS27" s="54"/>
+      <c r="AT27" s="54"/>
+      <c r="AU27" s="54"/>
+      <c r="AV27" s="54"/>
+      <c r="AW27" s="54"/>
+      <c r="AX27" s="54"/>
+      <c r="AY27" s="54"/>
+      <c r="AZ27" s="54"/>
+      <c r="BA27" s="54"/>
+      <c r="BB27" s="54"/>
+      <c r="BC27" s="54"/>
+      <c r="BD27" s="54"/>
+      <c r="BE27" s="54"/>
+      <c r="BF27" s="54"/>
+      <c r="BG27" s="54"/>
+      <c r="BH27" s="54"/>
+      <c r="BI27" s="54"/>
+      <c r="BJ27" s="54"/>
+      <c r="BK27" s="54"/>
+      <c r="BL27" s="54"/>
+      <c r="BM27" s="54"/>
+      <c r="BN27" s="54"/>
+      <c r="BO27" s="54"/>
     </row>
-    <row spans="1:67" r="28" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A28" s="27">
-        <v>3.1</v>
-      </c>
-      <c r="B28" s="73" t="s">
-        <v>45</v>
-      </c>
+    <row r="28" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A28" s="27"/>
+      <c r="B28" s="73"/>
       <c r="D28" s="74"/>
       <c r="E28" s="74"/>
-      <c r="F28" s="107"/>
+      <c r="F28" s="92"/>
       <c r="G28" s="51"/>
       <c r="H28" s="29"/>
       <c r="I28" s="30">
@@ -4440,92 +4421,96 @@
       <c r="BN28" s="54"/>
       <c r="BO28" s="54"/>
     </row>
-    <row spans="1:67" r="29" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A29" s="27"/>
-      <c r="B29" s="73"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="30">
-        <v>0</v>
-      </c>
-      <c r="J29" s="31" t="str">
-        <f t="shared" si="4"/>
+    <row r="29" spans="1:67" s="22" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="26" t="str">
+        <f t="shared" ref="J29:J36" si="5">IF(OR(G29=0,F29=0)," - ",NETWORKDAYS(F29,G29))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K29" s="48"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="54"/>
-      <c r="N29" s="54"/>
-      <c r="O29" s="54"/>
-      <c r="P29" s="54"/>
-      <c r="Q29" s="54"/>
-      <c r="R29" s="54"/>
-      <c r="S29" s="54"/>
-      <c r="T29" s="54"/>
-      <c r="U29" s="54"/>
-      <c r="V29" s="54"/>
-      <c r="W29" s="54"/>
-      <c r="X29" s="54"/>
-      <c r="Y29" s="54"/>
-      <c r="Z29" s="54"/>
-      <c r="AA29" s="54"/>
-      <c r="AB29" s="54"/>
-      <c r="AC29" s="54"/>
-      <c r="AD29" s="54"/>
-      <c r="AE29" s="54"/>
-      <c r="AF29" s="54"/>
-      <c r="AG29" s="54"/>
-      <c r="AH29" s="54"/>
-      <c r="AI29" s="54"/>
-      <c r="AJ29" s="54"/>
-      <c r="AK29" s="54"/>
-      <c r="AL29" s="54"/>
-      <c r="AM29" s="54"/>
-      <c r="AN29" s="54"/>
-      <c r="AO29" s="54"/>
-      <c r="AP29" s="54"/>
-      <c r="AQ29" s="54"/>
-      <c r="AR29" s="54"/>
-      <c r="AS29" s="54"/>
-      <c r="AT29" s="54"/>
-      <c r="AU29" s="54"/>
-      <c r="AV29" s="54"/>
-      <c r="AW29" s="54"/>
-      <c r="AX29" s="54"/>
-      <c r="AY29" s="54"/>
-      <c r="AZ29" s="54"/>
-      <c r="BA29" s="54"/>
-      <c r="BB29" s="54"/>
-      <c r="BC29" s="54"/>
-      <c r="BD29" s="54"/>
-      <c r="BE29" s="54"/>
-      <c r="BF29" s="54"/>
-      <c r="BG29" s="54"/>
-      <c r="BH29" s="54"/>
-      <c r="BI29" s="54"/>
-      <c r="BJ29" s="54"/>
-      <c r="BK29" s="54"/>
-      <c r="BL29" s="54"/>
-      <c r="BM29" s="54"/>
-      <c r="BN29" s="54"/>
-      <c r="BO29" s="54"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="56"/>
+      <c r="U29" s="56"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="56"/>
+      <c r="X29" s="56"/>
+      <c r="Y29" s="56"/>
+      <c r="Z29" s="56"/>
+      <c r="AA29" s="56"/>
+      <c r="AB29" s="56"/>
+      <c r="AC29" s="56"/>
+      <c r="AD29" s="56"/>
+      <c r="AE29" s="56"/>
+      <c r="AF29" s="56"/>
+      <c r="AG29" s="56"/>
+      <c r="AH29" s="56"/>
+      <c r="AI29" s="56"/>
+      <c r="AJ29" s="56"/>
+      <c r="AK29" s="56"/>
+      <c r="AL29" s="56"/>
+      <c r="AM29" s="56"/>
+      <c r="AN29" s="56"/>
+      <c r="AO29" s="56"/>
+      <c r="AP29" s="56"/>
+      <c r="AQ29" s="56"/>
+      <c r="AR29" s="56"/>
+      <c r="AS29" s="56"/>
+      <c r="AT29" s="56"/>
+      <c r="AU29" s="56"/>
+      <c r="AV29" s="56"/>
+      <c r="AW29" s="56"/>
+      <c r="AX29" s="56"/>
+      <c r="AY29" s="56"/>
+      <c r="AZ29" s="56"/>
+      <c r="BA29" s="56"/>
+      <c r="BB29" s="56"/>
+      <c r="BC29" s="56"/>
+      <c r="BD29" s="56"/>
+      <c r="BE29" s="56"/>
+      <c r="BF29" s="56"/>
+      <c r="BG29" s="56"/>
+      <c r="BH29" s="56"/>
+      <c r="BI29" s="56"/>
+      <c r="BJ29" s="56"/>
+      <c r="BK29" s="56"/>
+      <c r="BL29" s="56"/>
+      <c r="BM29" s="56"/>
+      <c r="BN29" s="56"/>
+      <c r="BO29" s="56"/>
     </row>
-    <row spans="1:67" r="30" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A30" s="27"/>
-      <c r="B30" s="73"/>
+    <row r="30" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A30" s="27">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B30" s="73" t="s">
+        <v>40</v>
+      </c>
       <c r="D30" s="74"/>
       <c r="E30" s="74"/>
-      <c r="F30" s="107"/>
+      <c r="F30" s="92"/>
       <c r="G30" s="51"/>
       <c r="H30" s="29"/>
       <c r="I30" s="30">
         <v>0</v>
       </c>
       <c r="J30" s="31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K30" s="48"/>
@@ -4586,19 +4571,19 @@
       <c r="BN30" s="54"/>
       <c r="BO30" s="54"/>
     </row>
-    <row spans="1:67" r="31" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="31" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
       <c r="B31" s="73"/>
       <c r="D31" s="74"/>
       <c r="E31" s="74"/>
-      <c r="F31" s="107"/>
+      <c r="F31" s="92"/>
       <c r="G31" s="51"/>
       <c r="H31" s="29"/>
       <c r="I31" s="30">
         <v>0</v>
       </c>
       <c r="J31" s="31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K31" s="48"/>
@@ -4659,19 +4644,19 @@
       <c r="BN31" s="54"/>
       <c r="BO31" s="54"/>
     </row>
-    <row spans="1:67" r="32" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="32" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="73"/>
       <c r="D32" s="74"/>
       <c r="E32" s="74"/>
-      <c r="F32" s="107"/>
+      <c r="F32" s="92"/>
       <c r="G32" s="51"/>
       <c r="H32" s="29"/>
       <c r="I32" s="30">
         <v>0</v>
       </c>
       <c r="J32" s="31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K32" s="48"/>
@@ -4732,92 +4717,88 @@
       <c r="BN32" s="54"/>
       <c r="BO32" s="54"/>
     </row>
-    <row spans="1:67" r="33" s="22" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A33" s="20"/>
-      <c r="B33" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="108"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="26" t="str">
-        <f ref="J33:J40" t="shared" si="5">IF(OR(G33=0,F33=0)," - ",NETWORKDAYS(F33,G33))</f>
+    <row r="33" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A33" s="27"/>
+      <c r="B33" s="73"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="92"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="30">
+        <v>0</v>
+      </c>
+      <c r="J33" s="31" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K33" s="49"/>
-      <c r="L33" s="56"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="56"/>
-      <c r="O33" s="56"/>
-      <c r="P33" s="56"/>
-      <c r="Q33" s="56"/>
-      <c r="R33" s="56"/>
-      <c r="S33" s="56"/>
-      <c r="T33" s="56"/>
-      <c r="U33" s="56"/>
-      <c r="V33" s="56"/>
-      <c r="W33" s="56"/>
-      <c r="X33" s="56"/>
-      <c r="Y33" s="56"/>
-      <c r="Z33" s="56"/>
-      <c r="AA33" s="56"/>
-      <c r="AB33" s="56"/>
-      <c r="AC33" s="56"/>
-      <c r="AD33" s="56"/>
-      <c r="AE33" s="56"/>
-      <c r="AF33" s="56"/>
-      <c r="AG33" s="56"/>
-      <c r="AH33" s="56"/>
-      <c r="AI33" s="56"/>
-      <c r="AJ33" s="56"/>
-      <c r="AK33" s="56"/>
-      <c r="AL33" s="56"/>
-      <c r="AM33" s="56"/>
-      <c r="AN33" s="56"/>
-      <c r="AO33" s="56"/>
-      <c r="AP33" s="56"/>
-      <c r="AQ33" s="56"/>
-      <c r="AR33" s="56"/>
-      <c r="AS33" s="56"/>
-      <c r="AT33" s="56"/>
-      <c r="AU33" s="56"/>
-      <c r="AV33" s="56"/>
-      <c r="AW33" s="56"/>
-      <c r="AX33" s="56"/>
-      <c r="AY33" s="56"/>
-      <c r="AZ33" s="56"/>
-      <c r="BA33" s="56"/>
-      <c r="BB33" s="56"/>
-      <c r="BC33" s="56"/>
-      <c r="BD33" s="56"/>
-      <c r="BE33" s="56"/>
-      <c r="BF33" s="56"/>
-      <c r="BG33" s="56"/>
-      <c r="BH33" s="56"/>
-      <c r="BI33" s="56"/>
-      <c r="BJ33" s="56"/>
-      <c r="BK33" s="56"/>
-      <c r="BL33" s="56"/>
-      <c r="BM33" s="56"/>
-      <c r="BN33" s="56"/>
-      <c r="BO33" s="56"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="54"/>
+      <c r="M33" s="54"/>
+      <c r="N33" s="54"/>
+      <c r="O33" s="54"/>
+      <c r="P33" s="54"/>
+      <c r="Q33" s="54"/>
+      <c r="R33" s="54"/>
+      <c r="S33" s="54"/>
+      <c r="T33" s="54"/>
+      <c r="U33" s="54"/>
+      <c r="V33" s="54"/>
+      <c r="W33" s="54"/>
+      <c r="X33" s="54"/>
+      <c r="Y33" s="54"/>
+      <c r="Z33" s="54"/>
+      <c r="AA33" s="54"/>
+      <c r="AB33" s="54"/>
+      <c r="AC33" s="54"/>
+      <c r="AD33" s="54"/>
+      <c r="AE33" s="54"/>
+      <c r="AF33" s="54"/>
+      <c r="AG33" s="54"/>
+      <c r="AH33" s="54"/>
+      <c r="AI33" s="54"/>
+      <c r="AJ33" s="54"/>
+      <c r="AK33" s="54"/>
+      <c r="AL33" s="54"/>
+      <c r="AM33" s="54"/>
+      <c r="AN33" s="54"/>
+      <c r="AO33" s="54"/>
+      <c r="AP33" s="54"/>
+      <c r="AQ33" s="54"/>
+      <c r="AR33" s="54"/>
+      <c r="AS33" s="54"/>
+      <c r="AT33" s="54"/>
+      <c r="AU33" s="54"/>
+      <c r="AV33" s="54"/>
+      <c r="AW33" s="54"/>
+      <c r="AX33" s="54"/>
+      <c r="AY33" s="54"/>
+      <c r="AZ33" s="54"/>
+      <c r="BA33" s="54"/>
+      <c r="BB33" s="54"/>
+      <c r="BC33" s="54"/>
+      <c r="BD33" s="54"/>
+      <c r="BE33" s="54"/>
+      <c r="BF33" s="54"/>
+      <c r="BG33" s="54"/>
+      <c r="BH33" s="54"/>
+      <c r="BI33" s="54"/>
+      <c r="BJ33" s="54"/>
+      <c r="BK33" s="54"/>
+      <c r="BL33" s="54"/>
+      <c r="BM33" s="54"/>
+      <c r="BN33" s="54"/>
+      <c r="BO33" s="54"/>
     </row>
-    <row spans="1:67" r="34" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A34" s="27">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B34" s="73" t="s">
-        <v>47</v>
-      </c>
+    <row r="34" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A34" s="27"/>
+      <c r="B34" s="73"/>
       <c r="D34" s="74"/>
       <c r="E34" s="74"/>
-      <c r="F34" s="107"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="30">
+      <c r="F34" s="96"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="99">
         <v>0</v>
       </c>
       <c r="J34" s="31" t="str">
@@ -4882,22 +4863,21 @@
       <c r="BN34" s="54"/>
       <c r="BO34" s="54"/>
     </row>
-    <row spans="1:67" r="35" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="35" spans="1:67" s="35" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A35" s="27"/>
-      <c r="B35" s="73"/>
-      <c r="D35" s="74"/>
-      <c r="E35" s="74"/>
-      <c r="F35" s="107"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="30">
-        <v>0</v>
-      </c>
-      <c r="J35" s="31" t="str">
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="101"/>
+      <c r="G35" s="102"/>
+      <c r="H35" s="103"/>
+      <c r="I35" s="104"/>
+      <c r="J35" s="34" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K35" s="48"/>
+      <c r="K35" s="50"/>
       <c r="L35" s="54"/>
       <c r="M35" s="54"/>
       <c r="N35" s="54"/>
@@ -4955,22 +4935,21 @@
       <c r="BN35" s="54"/>
       <c r="BO35" s="54"/>
     </row>
-    <row spans="1:67" r="36" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="36" spans="1:67" s="35" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A36" s="27"/>
-      <c r="B36" s="73"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="107"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="30">
-        <v>0</v>
-      </c>
-      <c r="J36" s="31" t="str">
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="101"/>
+      <c r="G36" s="102"/>
+      <c r="H36" s="103"/>
+      <c r="I36" s="104"/>
+      <c r="J36" s="34" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K36" s="48"/>
+      <c r="K36" s="50"/>
       <c r="L36" s="54"/>
       <c r="M36" s="54"/>
       <c r="N36" s="54"/>
@@ -5028,92 +5007,96 @@
       <c r="BN36" s="54"/>
       <c r="BO36" s="54"/>
     </row>
-    <row spans="1:67" r="37" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A37" s="27"/>
-      <c r="B37" s="73"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="107"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="30">
-        <v>0</v>
-      </c>
-      <c r="J37" s="31" t="str">
-        <f t="shared" si="5"/>
+    <row r="37" spans="1:67" s="22" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+      <c r="B37" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="26" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K37" s="48"/>
-      <c r="L37" s="54"/>
-      <c r="M37" s="54"/>
-      <c r="N37" s="54"/>
-      <c r="O37" s="54"/>
-      <c r="P37" s="54"/>
-      <c r="Q37" s="54"/>
-      <c r="R37" s="54"/>
-      <c r="S37" s="54"/>
-      <c r="T37" s="54"/>
-      <c r="U37" s="54"/>
-      <c r="V37" s="54"/>
-      <c r="W37" s="54"/>
-      <c r="X37" s="54"/>
-      <c r="Y37" s="54"/>
-      <c r="Z37" s="54"/>
-      <c r="AA37" s="54"/>
-      <c r="AB37" s="54"/>
-      <c r="AC37" s="54"/>
-      <c r="AD37" s="54"/>
-      <c r="AE37" s="54"/>
-      <c r="AF37" s="54"/>
-      <c r="AG37" s="54"/>
-      <c r="AH37" s="54"/>
-      <c r="AI37" s="54"/>
-      <c r="AJ37" s="54"/>
-      <c r="AK37" s="54"/>
-      <c r="AL37" s="54"/>
-      <c r="AM37" s="54"/>
-      <c r="AN37" s="54"/>
-      <c r="AO37" s="54"/>
-      <c r="AP37" s="54"/>
-      <c r="AQ37" s="54"/>
-      <c r="AR37" s="54"/>
-      <c r="AS37" s="54"/>
-      <c r="AT37" s="54"/>
-      <c r="AU37" s="54"/>
-      <c r="AV37" s="54"/>
-      <c r="AW37" s="54"/>
-      <c r="AX37" s="54"/>
-      <c r="AY37" s="54"/>
-      <c r="AZ37" s="54"/>
-      <c r="BA37" s="54"/>
-      <c r="BB37" s="54"/>
-      <c r="BC37" s="54"/>
-      <c r="BD37" s="54"/>
-      <c r="BE37" s="54"/>
-      <c r="BF37" s="54"/>
-      <c r="BG37" s="54"/>
-      <c r="BH37" s="54"/>
-      <c r="BI37" s="54"/>
-      <c r="BJ37" s="54"/>
-      <c r="BK37" s="54"/>
-      <c r="BL37" s="54"/>
-      <c r="BM37" s="54"/>
-      <c r="BN37" s="54"/>
-      <c r="BO37" s="54"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="56"/>
+      <c r="N37" s="56"/>
+      <c r="O37" s="56"/>
+      <c r="P37" s="56"/>
+      <c r="Q37" s="56"/>
+      <c r="R37" s="56"/>
+      <c r="S37" s="56"/>
+      <c r="T37" s="56"/>
+      <c r="U37" s="56"/>
+      <c r="V37" s="56"/>
+      <c r="W37" s="56"/>
+      <c r="X37" s="56"/>
+      <c r="Y37" s="56"/>
+      <c r="Z37" s="56"/>
+      <c r="AA37" s="56"/>
+      <c r="AB37" s="56"/>
+      <c r="AC37" s="56"/>
+      <c r="AD37" s="56"/>
+      <c r="AE37" s="56"/>
+      <c r="AF37" s="56"/>
+      <c r="AG37" s="56"/>
+      <c r="AH37" s="56"/>
+      <c r="AI37" s="56"/>
+      <c r="AJ37" s="56"/>
+      <c r="AK37" s="56"/>
+      <c r="AL37" s="56"/>
+      <c r="AM37" s="56"/>
+      <c r="AN37" s="56"/>
+      <c r="AO37" s="56"/>
+      <c r="AP37" s="56"/>
+      <c r="AQ37" s="56"/>
+      <c r="AR37" s="56"/>
+      <c r="AS37" s="56"/>
+      <c r="AT37" s="56"/>
+      <c r="AU37" s="56"/>
+      <c r="AV37" s="56"/>
+      <c r="AW37" s="56"/>
+      <c r="AX37" s="56"/>
+      <c r="AY37" s="56"/>
+      <c r="AZ37" s="56"/>
+      <c r="BA37" s="56"/>
+      <c r="BB37" s="56"/>
+      <c r="BC37" s="56"/>
+      <c r="BD37" s="56"/>
+      <c r="BE37" s="56"/>
+      <c r="BF37" s="56"/>
+      <c r="BG37" s="56"/>
+      <c r="BH37" s="56"/>
+      <c r="BI37" s="56"/>
+      <c r="BJ37" s="56"/>
+      <c r="BK37" s="56"/>
+      <c r="BL37" s="56"/>
+      <c r="BM37" s="56"/>
+      <c r="BN37" s="56"/>
+      <c r="BO37" s="56"/>
     </row>
-    <row spans="1:67" r="38" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A38" s="27"/>
-      <c r="B38" s="73"/>
+    <row r="38" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A38" s="27">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B38" s="73" t="s">
+        <v>42</v>
+      </c>
       <c r="D38" s="74"/>
       <c r="E38" s="74"/>
-      <c r="F38" s="111"/>
-      <c r="G38" s="112"/>
-      <c r="H38" s="113"/>
-      <c r="I38" s="114">
+      <c r="F38" s="92"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="30">
         <v>0</v>
       </c>
       <c r="J38" s="31" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K38" s="48"/>
@@ -5174,21 +5157,22 @@
       <c r="BN38" s="54"/>
       <c r="BO38" s="54"/>
     </row>
-    <row spans="1:67" r="39" s="35" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="39" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A39" s="27"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="116"/>
-      <c r="G39" s="117"/>
-      <c r="H39" s="118"/>
-      <c r="I39" s="119"/>
-      <c r="J39" s="34" t="str">
-        <f t="shared" si="5"/>
+      <c r="B39" s="73"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="30">
+        <v>0</v>
+      </c>
+      <c r="J39" s="31" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K39" s="50"/>
+      <c r="K39" s="48"/>
       <c r="L39" s="54"/>
       <c r="M39" s="54"/>
       <c r="N39" s="54"/>
@@ -5246,21 +5230,22 @@
       <c r="BN39" s="54"/>
       <c r="BO39" s="54"/>
     </row>
-    <row spans="1:67" r="40" s="35" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="40" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A40" s="27"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="116"/>
-      <c r="G40" s="117"/>
-      <c r="H40" s="118"/>
-      <c r="I40" s="119"/>
-      <c r="J40" s="34" t="str">
-        <f t="shared" si="5"/>
+      <c r="B40" s="73"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="92"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="30">
+        <v>0</v>
+      </c>
+      <c r="J40" s="31" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K40" s="50"/>
+      <c r="K40" s="48"/>
       <c r="L40" s="54"/>
       <c r="M40" s="54"/>
       <c r="N40" s="54"/>
@@ -5318,89 +5303,85 @@
       <c r="BN40" s="54"/>
       <c r="BO40" s="54"/>
     </row>
-    <row spans="1:67" r="41" s="22" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A41" s="20"/>
-      <c r="B41" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="115"/>
-      <c r="G41" s="62"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="26" t="str">
+    <row r="41" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A41" s="27"/>
+      <c r="B41" s="73"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="92"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="30">
+        <v>0</v>
+      </c>
+      <c r="J41" s="31" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K41" s="49"/>
-      <c r="L41" s="56"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="56"/>
-      <c r="O41" s="56"/>
-      <c r="P41" s="56"/>
-      <c r="Q41" s="56"/>
-      <c r="R41" s="56"/>
-      <c r="S41" s="56"/>
-      <c r="T41" s="56"/>
-      <c r="U41" s="56"/>
-      <c r="V41" s="56"/>
-      <c r="W41" s="56"/>
-      <c r="X41" s="56"/>
-      <c r="Y41" s="56"/>
-      <c r="Z41" s="56"/>
-      <c r="AA41" s="56"/>
-      <c r="AB41" s="56"/>
-      <c r="AC41" s="56"/>
-      <c r="AD41" s="56"/>
-      <c r="AE41" s="56"/>
-      <c r="AF41" s="56"/>
-      <c r="AG41" s="56"/>
-      <c r="AH41" s="56"/>
-      <c r="AI41" s="56"/>
-      <c r="AJ41" s="56"/>
-      <c r="AK41" s="56"/>
-      <c r="AL41" s="56"/>
-      <c r="AM41" s="56"/>
-      <c r="AN41" s="56"/>
-      <c r="AO41" s="56"/>
-      <c r="AP41" s="56"/>
-      <c r="AQ41" s="56"/>
-      <c r="AR41" s="56"/>
-      <c r="AS41" s="56"/>
-      <c r="AT41" s="56"/>
-      <c r="AU41" s="56"/>
-      <c r="AV41" s="56"/>
-      <c r="AW41" s="56"/>
-      <c r="AX41" s="56"/>
-      <c r="AY41" s="56"/>
-      <c r="AZ41" s="56"/>
-      <c r="BA41" s="56"/>
-      <c r="BB41" s="56"/>
-      <c r="BC41" s="56"/>
-      <c r="BD41" s="56"/>
-      <c r="BE41" s="56"/>
-      <c r="BF41" s="56"/>
-      <c r="BG41" s="56"/>
-      <c r="BH41" s="56"/>
-      <c r="BI41" s="56"/>
-      <c r="BJ41" s="56"/>
-      <c r="BK41" s="56"/>
-      <c r="BL41" s="56"/>
-      <c r="BM41" s="56"/>
-      <c r="BN41" s="56"/>
-      <c r="BO41" s="56"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="54"/>
+      <c r="M41" s="54"/>
+      <c r="N41" s="54"/>
+      <c r="O41" s="54"/>
+      <c r="P41" s="54"/>
+      <c r="Q41" s="54"/>
+      <c r="R41" s="54"/>
+      <c r="S41" s="54"/>
+      <c r="T41" s="54"/>
+      <c r="U41" s="54"/>
+      <c r="V41" s="54"/>
+      <c r="W41" s="54"/>
+      <c r="X41" s="54"/>
+      <c r="Y41" s="54"/>
+      <c r="Z41" s="54"/>
+      <c r="AA41" s="54"/>
+      <c r="AB41" s="54"/>
+      <c r="AC41" s="54"/>
+      <c r="AD41" s="54"/>
+      <c r="AE41" s="54"/>
+      <c r="AF41" s="54"/>
+      <c r="AG41" s="54"/>
+      <c r="AH41" s="54"/>
+      <c r="AI41" s="54"/>
+      <c r="AJ41" s="54"/>
+      <c r="AK41" s="54"/>
+      <c r="AL41" s="54"/>
+      <c r="AM41" s="54"/>
+      <c r="AN41" s="54"/>
+      <c r="AO41" s="54"/>
+      <c r="AP41" s="54"/>
+      <c r="AQ41" s="54"/>
+      <c r="AR41" s="54"/>
+      <c r="AS41" s="54"/>
+      <c r="AT41" s="54"/>
+      <c r="AU41" s="54"/>
+      <c r="AV41" s="54"/>
+      <c r="AW41" s="54"/>
+      <c r="AX41" s="54"/>
+      <c r="AY41" s="54"/>
+      <c r="AZ41" s="54"/>
+      <c r="BA41" s="54"/>
+      <c r="BB41" s="54"/>
+      <c r="BC41" s="54"/>
+      <c r="BD41" s="54"/>
+      <c r="BE41" s="54"/>
+      <c r="BF41" s="54"/>
+      <c r="BG41" s="54"/>
+      <c r="BH41" s="54"/>
+      <c r="BI41" s="54"/>
+      <c r="BJ41" s="54"/>
+      <c r="BK41" s="54"/>
+      <c r="BL41" s="54"/>
+      <c r="BM41" s="54"/>
+      <c r="BN41" s="54"/>
+      <c r="BO41" s="54"/>
     </row>
-    <row spans="1:67" r="42" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A42" s="27">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B42" s="73" t="s">
-        <v>49</v>
-      </c>
+    <row r="42" spans="1:67" s="28" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A42" s="27"/>
+      <c r="B42" s="73"/>
       <c r="D42" s="74"/>
       <c r="E42" s="74"/>
-      <c r="F42" s="107"/>
+      <c r="F42" s="92"/>
       <c r="G42" s="51"/>
       <c r="H42" s="29"/>
       <c r="I42" s="30">
@@ -5468,22 +5449,21 @@
       <c r="BN42" s="54"/>
       <c r="BO42" s="54"/>
     </row>
-    <row spans="1:67" r="43" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="43" spans="1:67" s="35" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A43" s="27"/>
-      <c r="B43" s="73"/>
-      <c r="D43" s="74"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="107"/>
-      <c r="G43" s="51"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="30">
-        <v>0</v>
-      </c>
-      <c r="J43" s="31" t="str">
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="94"/>
+      <c r="G43" s="78"/>
+      <c r="H43" s="79"/>
+      <c r="I43" s="80"/>
+      <c r="J43" s="34" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K43" s="48"/>
+      <c r="K43" s="50"/>
       <c r="L43" s="54"/>
       <c r="M43" s="54"/>
       <c r="N43" s="54"/>
@@ -5541,22 +5521,21 @@
       <c r="BN43" s="54"/>
       <c r="BO43" s="54"/>
     </row>
-    <row spans="1:67" r="44" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
+    <row r="44" spans="1:67" s="35" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A44" s="27"/>
-      <c r="B44" s="73"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="107"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="30">
-        <v>0</v>
-      </c>
-      <c r="J44" s="31" t="str">
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="94"/>
+      <c r="G44" s="78"/>
+      <c r="H44" s="79"/>
+      <c r="I44" s="80"/>
+      <c r="J44" s="34" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K44" s="48"/>
+      <c r="K44" s="50"/>
       <c r="L44" s="54"/>
       <c r="M44" s="54"/>
       <c r="N44" s="54"/>
@@ -5614,22 +5593,18 @@
       <c r="BN44" s="54"/>
       <c r="BO44" s="54"/>
     </row>
-    <row spans="1:67" r="45" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A45" s="27"/>
-      <c r="B45" s="73"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="74"/>
-      <c r="F45" s="107"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="30">
-        <v>0</v>
-      </c>
-      <c r="J45" s="31" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K45" s="48"/>
+    <row r="45" spans="1:67" s="36" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A45" s="54"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="54"/>
+      <c r="K45" s="54"/>
       <c r="L45" s="54"/>
       <c r="M45" s="54"/>
       <c r="N45" s="54"/>
@@ -5674,35 +5649,19 @@
       <c r="BA45" s="54"/>
       <c r="BB45" s="54"/>
       <c r="BC45" s="54"/>
-      <c r="BD45" s="54"/>
-      <c r="BE45" s="54"/>
-      <c r="BF45" s="54"/>
-      <c r="BG45" s="54"/>
-      <c r="BH45" s="54"/>
-      <c r="BI45" s="54"/>
-      <c r="BJ45" s="54"/>
-      <c r="BK45" s="54"/>
-      <c r="BL45" s="54"/>
-      <c r="BM45" s="54"/>
-      <c r="BN45" s="54"/>
-      <c r="BO45" s="54"/>
     </row>
-    <row spans="1:67" r="46" s="28" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A46" s="27"/>
-      <c r="B46" s="73"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="107"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="30">
-        <v>0</v>
-      </c>
-      <c r="J46" s="31" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K46" s="48"/>
+    <row r="46" spans="1:67" s="35" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A46" s="54"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="54"/>
+      <c r="I46" s="54"/>
+      <c r="J46" s="54"/>
+      <c r="K46" s="54"/>
       <c r="L46" s="54"/>
       <c r="M46" s="54"/>
       <c r="N46" s="54"/>
@@ -5747,34 +5706,19 @@
       <c r="BA46" s="54"/>
       <c r="BB46" s="54"/>
       <c r="BC46" s="54"/>
-      <c r="BD46" s="54"/>
-      <c r="BE46" s="54"/>
-      <c r="BF46" s="54"/>
-      <c r="BG46" s="54"/>
-      <c r="BH46" s="54"/>
-      <c r="BI46" s="54"/>
-      <c r="BJ46" s="54"/>
-      <c r="BK46" s="54"/>
-      <c r="BL46" s="54"/>
-      <c r="BM46" s="54"/>
-      <c r="BN46" s="54"/>
-      <c r="BO46" s="54"/>
     </row>
-    <row spans="1:67" r="47" s="35" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A47" s="27"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="109"/>
-      <c r="G47" s="78"/>
-      <c r="H47" s="79"/>
-      <c r="I47" s="80"/>
-      <c r="J47" s="34" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K47" s="50"/>
+    <row r="47" spans="1:67" s="35" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A47" s="54"/>
+      <c r="B47" s="54"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="54"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="54"/>
+      <c r="K47" s="54"/>
       <c r="L47" s="54"/>
       <c r="M47" s="54"/>
       <c r="N47" s="54"/>
@@ -5819,34 +5763,19 @@
       <c r="BA47" s="54"/>
       <c r="BB47" s="54"/>
       <c r="BC47" s="54"/>
-      <c r="BD47" s="54"/>
-      <c r="BE47" s="54"/>
-      <c r="BF47" s="54"/>
-      <c r="BG47" s="54"/>
-      <c r="BH47" s="54"/>
-      <c r="BI47" s="54"/>
-      <c r="BJ47" s="54"/>
-      <c r="BK47" s="54"/>
-      <c r="BL47" s="54"/>
-      <c r="BM47" s="54"/>
-      <c r="BN47" s="54"/>
-      <c r="BO47" s="54"/>
     </row>
-    <row spans="1:67" r="48" s="35" x14ac:dyDescent="0.25" ht="17.399999999999999" customFormat="1">
-      <c r="A48" s="27"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="109"/>
-      <c r="G48" s="78"/>
-      <c r="H48" s="79"/>
-      <c r="I48" s="80"/>
-      <c r="J48" s="34" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K48" s="50"/>
+    <row r="48" spans="1:67" s="35" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
+      <c r="A48" s="54"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="54"/>
+      <c r="I48" s="54"/>
+      <c r="J48" s="54"/>
+      <c r="K48" s="54"/>
       <c r="L48" s="54"/>
       <c r="M48" s="54"/>
       <c r="N48" s="54"/>
@@ -5891,20 +5820,8 @@
       <c r="BA48" s="54"/>
       <c r="BB48" s="54"/>
       <c r="BC48" s="54"/>
-      <c r="BD48" s="54"/>
-      <c r="BE48" s="54"/>
-      <c r="BF48" s="54"/>
-      <c r="BG48" s="54"/>
-      <c r="BH48" s="54"/>
-      <c r="BI48" s="54"/>
-      <c r="BJ48" s="54"/>
-      <c r="BK48" s="54"/>
-      <c r="BL48" s="54"/>
-      <c r="BM48" s="54"/>
-      <c r="BN48" s="54"/>
-      <c r="BO48" s="54"/>
     </row>
-    <row spans="1:67" r="49" s="36" x14ac:dyDescent="0.25" ht="11.4" customFormat="1">
+    <row r="49" spans="1:67" s="35" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
       <c r="A49" s="54"/>
       <c r="B49" s="54"/>
       <c r="C49" s="54"/>
@@ -5961,7 +5878,7 @@
       <c r="BB49" s="54"/>
       <c r="BC49" s="54"/>
     </row>
-    <row spans="1:67" r="50" s="35" x14ac:dyDescent="0.25" ht="11.4" customFormat="1">
+    <row r="50" spans="1:67" s="35" customFormat="1" ht="11.4" x14ac:dyDescent="0.25">
       <c r="A50" s="54"/>
       <c r="B50" s="54"/>
       <c r="C50" s="54"/>
@@ -6018,317 +5935,89 @@
       <c r="BB50" s="54"/>
       <c r="BC50" s="54"/>
     </row>
-    <row spans="1:67" r="51" s="35" x14ac:dyDescent="0.25" ht="11.4" customFormat="1">
-      <c r="A51" s="54"/>
-      <c r="B51" s="54"/>
-      <c r="C51" s="54"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="54"/>
-      <c r="H51" s="54"/>
-      <c r="I51" s="54"/>
-      <c r="J51" s="54"/>
-      <c r="K51" s="54"/>
-      <c r="L51" s="54"/>
-      <c r="M51" s="54"/>
-      <c r="N51" s="54"/>
-      <c r="O51" s="54"/>
-      <c r="P51" s="54"/>
-      <c r="Q51" s="54"/>
-      <c r="R51" s="54"/>
-      <c r="S51" s="54"/>
-      <c r="T51" s="54"/>
-      <c r="U51" s="54"/>
-      <c r="V51" s="54"/>
-      <c r="W51" s="54"/>
-      <c r="X51" s="54"/>
-      <c r="Y51" s="54"/>
-      <c r="Z51" s="54"/>
-      <c r="AA51" s="54"/>
-      <c r="AB51" s="54"/>
-      <c r="AC51" s="54"/>
-      <c r="AD51" s="54"/>
-      <c r="AE51" s="54"/>
-      <c r="AF51" s="54"/>
-      <c r="AG51" s="54"/>
-      <c r="AH51" s="54"/>
-      <c r="AI51" s="54"/>
-      <c r="AJ51" s="54"/>
-      <c r="AK51" s="54"/>
-      <c r="AL51" s="54"/>
-      <c r="AM51" s="54"/>
-      <c r="AN51" s="54"/>
-      <c r="AO51" s="54"/>
-      <c r="AP51" s="54"/>
-      <c r="AQ51" s="54"/>
-      <c r="AR51" s="54"/>
-      <c r="AS51" s="54"/>
-      <c r="AT51" s="54"/>
-      <c r="AU51" s="54"/>
-      <c r="AV51" s="54"/>
-      <c r="AW51" s="54"/>
-      <c r="AX51" s="54"/>
-      <c r="AY51" s="54"/>
-      <c r="AZ51" s="54"/>
-      <c r="BA51" s="54"/>
-      <c r="BB51" s="54"/>
-      <c r="BC51" s="54"/>
-    </row>
-    <row spans="1:67" r="52" s="35" x14ac:dyDescent="0.25" ht="11.4" customFormat="1">
-      <c r="A52" s="54"/>
-      <c r="B52" s="54"/>
-      <c r="C52" s="54"/>
-      <c r="D52" s="54"/>
-      <c r="E52" s="54"/>
-      <c r="F52" s="54"/>
-      <c r="G52" s="54"/>
-      <c r="H52" s="54"/>
-      <c r="I52" s="54"/>
-      <c r="J52" s="54"/>
-      <c r="K52" s="54"/>
-      <c r="L52" s="54"/>
-      <c r="M52" s="54"/>
-      <c r="N52" s="54"/>
-      <c r="O52" s="54"/>
-      <c r="P52" s="54"/>
-      <c r="Q52" s="54"/>
-      <c r="R52" s="54"/>
-      <c r="S52" s="54"/>
-      <c r="T52" s="54"/>
-      <c r="U52" s="54"/>
-      <c r="V52" s="54"/>
-      <c r="W52" s="54"/>
-      <c r="X52" s="54"/>
-      <c r="Y52" s="54"/>
-      <c r="Z52" s="54"/>
-      <c r="AA52" s="54"/>
-      <c r="AB52" s="54"/>
-      <c r="AC52" s="54"/>
-      <c r="AD52" s="54"/>
-      <c r="AE52" s="54"/>
-      <c r="AF52" s="54"/>
-      <c r="AG52" s="54"/>
-      <c r="AH52" s="54"/>
-      <c r="AI52" s="54"/>
-      <c r="AJ52" s="54"/>
-      <c r="AK52" s="54"/>
-      <c r="AL52" s="54"/>
-      <c r="AM52" s="54"/>
-      <c r="AN52" s="54"/>
-      <c r="AO52" s="54"/>
-      <c r="AP52" s="54"/>
-      <c r="AQ52" s="54"/>
-      <c r="AR52" s="54"/>
-      <c r="AS52" s="54"/>
-      <c r="AT52" s="54"/>
-      <c r="AU52" s="54"/>
-      <c r="AV52" s="54"/>
-      <c r="AW52" s="54"/>
-      <c r="AX52" s="54"/>
-      <c r="AY52" s="54"/>
-      <c r="AZ52" s="54"/>
-      <c r="BA52" s="54"/>
-      <c r="BB52" s="54"/>
-      <c r="BC52" s="54"/>
-    </row>
-    <row spans="1:67" r="53" s="35" x14ac:dyDescent="0.25" ht="11.4" customFormat="1">
-      <c r="A53" s="54"/>
-      <c r="B53" s="54"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="54"/>
-      <c r="E53" s="54"/>
-      <c r="F53" s="54"/>
-      <c r="G53" s="54"/>
-      <c r="H53" s="54"/>
-      <c r="I53" s="54"/>
-      <c r="J53" s="54"/>
-      <c r="K53" s="54"/>
-      <c r="L53" s="54"/>
-      <c r="M53" s="54"/>
-      <c r="N53" s="54"/>
-      <c r="O53" s="54"/>
-      <c r="P53" s="54"/>
-      <c r="Q53" s="54"/>
-      <c r="R53" s="54"/>
-      <c r="S53" s="54"/>
-      <c r="T53" s="54"/>
-      <c r="U53" s="54"/>
-      <c r="V53" s="54"/>
-      <c r="W53" s="54"/>
-      <c r="X53" s="54"/>
-      <c r="Y53" s="54"/>
-      <c r="Z53" s="54"/>
-      <c r="AA53" s="54"/>
-      <c r="AB53" s="54"/>
-      <c r="AC53" s="54"/>
-      <c r="AD53" s="54"/>
-      <c r="AE53" s="54"/>
-      <c r="AF53" s="54"/>
-      <c r="AG53" s="54"/>
-      <c r="AH53" s="54"/>
-      <c r="AI53" s="54"/>
-      <c r="AJ53" s="54"/>
-      <c r="AK53" s="54"/>
-      <c r="AL53" s="54"/>
-      <c r="AM53" s="54"/>
-      <c r="AN53" s="54"/>
-      <c r="AO53" s="54"/>
-      <c r="AP53" s="54"/>
-      <c r="AQ53" s="54"/>
-      <c r="AR53" s="54"/>
-      <c r="AS53" s="54"/>
-      <c r="AT53" s="54"/>
-      <c r="AU53" s="54"/>
-      <c r="AV53" s="54"/>
-      <c r="AW53" s="54"/>
-      <c r="AX53" s="54"/>
-      <c r="AY53" s="54"/>
-      <c r="AZ53" s="54"/>
-      <c r="BA53" s="54"/>
-      <c r="BB53" s="54"/>
-      <c r="BC53" s="54"/>
-    </row>
-    <row spans="1:67" r="54" s="35" x14ac:dyDescent="0.25" ht="11.4" customFormat="1">
-      <c r="A54" s="54"/>
-      <c r="B54" s="54"/>
-      <c r="C54" s="54"/>
-      <c r="D54" s="54"/>
-      <c r="E54" s="54"/>
-      <c r="F54" s="54"/>
-      <c r="G54" s="54"/>
-      <c r="H54" s="54"/>
-      <c r="I54" s="54"/>
-      <c r="J54" s="54"/>
-      <c r="K54" s="54"/>
-      <c r="L54" s="54"/>
-      <c r="M54" s="54"/>
-      <c r="N54" s="54"/>
-      <c r="O54" s="54"/>
-      <c r="P54" s="54"/>
-      <c r="Q54" s="54"/>
-      <c r="R54" s="54"/>
-      <c r="S54" s="54"/>
-      <c r="T54" s="54"/>
-      <c r="U54" s="54"/>
-      <c r="V54" s="54"/>
-      <c r="W54" s="54"/>
-      <c r="X54" s="54"/>
-      <c r="Y54" s="54"/>
-      <c r="Z54" s="54"/>
-      <c r="AA54" s="54"/>
-      <c r="AB54" s="54"/>
-      <c r="AC54" s="54"/>
-      <c r="AD54" s="54"/>
-      <c r="AE54" s="54"/>
-      <c r="AF54" s="54"/>
-      <c r="AG54" s="54"/>
-      <c r="AH54" s="54"/>
-      <c r="AI54" s="54"/>
-      <c r="AJ54" s="54"/>
-      <c r="AK54" s="54"/>
-      <c r="AL54" s="54"/>
-      <c r="AM54" s="54"/>
-      <c r="AN54" s="54"/>
-      <c r="AO54" s="54"/>
-      <c r="AP54" s="54"/>
-      <c r="AQ54" s="54"/>
-      <c r="AR54" s="54"/>
-      <c r="AS54" s="54"/>
-      <c r="AT54" s="54"/>
-      <c r="AU54" s="54"/>
-      <c r="AV54" s="54"/>
-      <c r="AW54" s="54"/>
-      <c r="AX54" s="54"/>
-      <c r="AY54" s="54"/>
-      <c r="AZ54" s="54"/>
-      <c r="BA54" s="54"/>
-      <c r="BB54" s="54"/>
-      <c r="BC54" s="54"/>
-    </row>
-    <row spans="1:67" r="55" s="12" x14ac:dyDescent="0.25" customFormat="1">
-      <c r="A55" s="9"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
-      <c r="L55" s="10"/>
-      <c r="M55" s="10"/>
-      <c r="N55" s="10"/>
-      <c r="O55" s="10"/>
-      <c r="P55" s="10"/>
-      <c r="Q55" s="10"/>
-      <c r="R55" s="10"/>
-      <c r="S55" s="10"/>
-      <c r="T55" s="10"/>
-      <c r="U55" s="10"/>
-      <c r="V55" s="10"/>
-      <c r="W55" s="10"/>
-      <c r="X55" s="10"/>
-      <c r="Y55" s="10"/>
-      <c r="Z55" s="10"/>
-      <c r="AA55" s="10"/>
-      <c r="AB55" s="10"/>
-      <c r="AC55" s="10"/>
-      <c r="AD55" s="10"/>
-      <c r="AE55" s="10"/>
-      <c r="AF55" s="10"/>
-      <c r="AG55" s="10"/>
-      <c r="AH55" s="10"/>
-      <c r="AI55" s="10"/>
-      <c r="AJ55" s="10"/>
-      <c r="AK55" s="10"/>
-      <c r="AL55" s="10"/>
-      <c r="AM55" s="10"/>
-      <c r="AN55" s="10"/>
-      <c r="AO55" s="10"/>
-      <c r="AP55" s="10"/>
-      <c r="AQ55" s="10"/>
-      <c r="AR55" s="10"/>
-      <c r="AS55" s="10"/>
-      <c r="AT55" s="10"/>
-      <c r="AU55" s="10"/>
-      <c r="AV55" s="10"/>
-      <c r="AW55" s="10"/>
-      <c r="AX55" s="10"/>
-      <c r="AY55" s="10"/>
-      <c r="AZ55" s="10"/>
-      <c r="BA55" s="10"/>
-      <c r="BB55" s="10"/>
-      <c r="BC55" s="10"/>
-      <c r="BD55" s="10"/>
-      <c r="BE55" s="10"/>
-      <c r="BF55" s="10"/>
-      <c r="BG55" s="10"/>
-      <c r="BH55" s="10"/>
-      <c r="BI55" s="10"/>
-      <c r="BJ55" s="10"/>
-      <c r="BK55" s="10"/>
-      <c r="BL55" s="10"/>
-      <c r="BM55" s="10"/>
-      <c r="BN55" s="10"/>
-      <c r="BO55" s="10"/>
+    <row r="51" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="9"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="10"/>
+      <c r="S51" s="10"/>
+      <c r="T51" s="10"/>
+      <c r="U51" s="10"/>
+      <c r="V51" s="10"/>
+      <c r="W51" s="10"/>
+      <c r="X51" s="10"/>
+      <c r="Y51" s="10"/>
+      <c r="Z51" s="10"/>
+      <c r="AA51" s="10"/>
+      <c r="AB51" s="10"/>
+      <c r="AC51" s="10"/>
+      <c r="AD51" s="10"/>
+      <c r="AE51" s="10"/>
+      <c r="AF51" s="10"/>
+      <c r="AG51" s="10"/>
+      <c r="AH51" s="10"/>
+      <c r="AI51" s="10"/>
+      <c r="AJ51" s="10"/>
+      <c r="AK51" s="10"/>
+      <c r="AL51" s="10"/>
+      <c r="AM51" s="10"/>
+      <c r="AN51" s="10"/>
+      <c r="AO51" s="10"/>
+      <c r="AP51" s="10"/>
+      <c r="AQ51" s="10"/>
+      <c r="AR51" s="10"/>
+      <c r="AS51" s="10"/>
+      <c r="AT51" s="10"/>
+      <c r="AU51" s="10"/>
+      <c r="AV51" s="10"/>
+      <c r="AW51" s="10"/>
+      <c r="AX51" s="10"/>
+      <c r="AY51" s="10"/>
+      <c r="AZ51" s="10"/>
+      <c r="BA51" s="10"/>
+      <c r="BB51" s="10"/>
+      <c r="BC51" s="10"/>
+      <c r="BD51" s="10"/>
+      <c r="BE51" s="10"/>
+      <c r="BF51" s="10"/>
+      <c r="BG51" s="10"/>
+      <c r="BH51" s="10"/>
+      <c r="BI51" s="10"/>
+      <c r="BJ51" s="10"/>
+      <c r="BK51" s="10"/>
+      <c r="BL51" s="10"/>
+      <c r="BM51" s="10"/>
+      <c r="BN51" s="10"/>
+      <c r="BO51" s="10"/>
     </row>
   </sheetData>
-  <sheetProtection formatColumns="0" formatCells="0" insertRows="0" deleteRows="0" formatRows="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="BI5:BO5"/>
-    <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="BI4:BO4"/>
-    <mergeCell ref="BB4:BH4"/>
-    <mergeCell ref="L1:AF1"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="S4:Y4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="S5:Y5"/>
     <mergeCell ref="L5:R5"/>
+    <mergeCell ref="BI5:BO5"/>
+    <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="BI4:BO4"/>
+    <mergeCell ref="BB4:BH4"/>
+    <mergeCell ref="L1:AF1"/>
     <mergeCell ref="Z4:AF4"/>
     <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
@@ -6339,11 +6028,11 @@
     <mergeCell ref="AN4:AT4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I32 I41:I48">
+  <conditionalFormatting sqref="I37:I44 I8:I28">
     <cfRule type="dataBar" priority="10">
       <dataBar>
-        <cfvo val="0" type="num"/>
-        <cfvo val="1" type="num"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
       <extLst>
@@ -6354,41 +6043,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:BO7">
-    <cfRule dxfId="12" type="expression" priority="53">
+    <cfRule type="expression" dxfId="7" priority="53">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO17 L19:BO32 L41:BO48">
-    <cfRule dxfId="11" type="expression" priority="56">
+  <conditionalFormatting sqref="L8:BO44">
+    <cfRule type="expression" dxfId="6" priority="56">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule dxfId="10" type="expression" priority="57">
+    <cfRule type="expression" dxfId="5" priority="57">
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO17 L19:BO32 L41:BO48">
-    <cfRule dxfId="9" type="expression" priority="16">
+  <conditionalFormatting sqref="L37:BO44 L6:BO28">
+    <cfRule type="expression" dxfId="4" priority="16">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L18:BO18">
-    <cfRule dxfId="8" type="expression" priority="7">
-      <formula>AND($F18&lt;=L$6,ROUNDDOWN(($G18-$F18+1)*$I18,0)+$F18-1&gt;=L$6)</formula>
-    </cfRule>
-    <cfRule dxfId="7" type="expression" priority="8">
-      <formula>AND(NOT(ISBLANK($F18)),$F18&lt;=L$6,$G18&gt;=L$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L18:BO18">
-    <cfRule dxfId="6" type="expression" priority="6">
-      <formula>L$6=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33:I40">
+  <conditionalFormatting sqref="I29:I36">
     <cfRule type="dataBar" priority="1">
       <dataBar>
-        <cfvo val="0" type="num"/>
-        <cfvo val="1" type="num"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
       <extLst>
@@ -6398,43 +6074,35 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L33:BO40">
-    <cfRule dxfId="5" type="expression" priority="3">
-      <formula>AND($F33&lt;=L$6,ROUNDDOWN(($G33-$F33+1)*$I33,0)+$F33-1&gt;=L$6)</formula>
-    </cfRule>
-    <cfRule dxfId="4" type="expression" priority="4">
-      <formula>AND(NOT(ISBLANK($F33)),$F33&lt;=L$6,$G33&gt;=L$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L33:BO40">
-    <cfRule dxfId="3" type="expression" priority="2">
+  <conditionalFormatting sqref="L29:BO36">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49:BC54">
-    <cfRule dxfId="2" type="expression" priority="60">
+  <conditionalFormatting sqref="A45:BC50">
+    <cfRule type="expression" dxfId="2" priority="60">
       <formula>AND(#REF!&lt;=M$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=M$6)</formula>
     </cfRule>
-    <cfRule dxfId="1" type="expression" priority="61">
+    <cfRule type="expression" dxfId="1" priority="61">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=M$6,#REF!&gt;=M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49:BC54">
-    <cfRule dxfId="0" type="expression" priority="63">
+  <conditionalFormatting sqref="A45:BC50">
+    <cfRule type="expression" dxfId="0" priority="63">
       <formula>M$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Display Week" sqref="I4" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Project Start Date."/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Project Start Date." sqref="I4"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="L1:AF1" display="Gantt Chart Template © 2006-2018 by Vertex42.com." r:id="rId1"/>
+    <hyperlink ref="L1:AF1" r:id="rId1" display="Gantt Chart Template © 2006-2018 by Vertex42.com."/>
   </hyperlinks>
-  <pageMargins top="0.5" left="0.25" footer="0.25" bottom="0.5" header="0.5" right="0.25"/>
-  <pageSetup orientation="landscape" fitToHeight="0" scale="63" r:id="rId2"/>
+  <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.25"/>
+  <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError unlockedFormula="1" sqref="A47:B48 F47:I48 H21:I21 H27:I27 H41:I41 I25 I23 I24 I28:I31 I42:I45"/>
+    <ignoredError sqref="A43:B44 F43:I44 H17:I17 H23:I23 H37:I37 I21 I19 I20 I24:I27 I38:I41" unlockedFormula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -6443,8 +6111,8 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="8238" name="Scroll Bar 46" r:id="rId5">
-              <controlPr print="0" defaultSize="0" autoPict="0">
+            <control shapeId="9262" r:id="rId5" name="Scroll Bar 46">
+              <controlPr defaultSize="0" print="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
@@ -6470,8 +6138,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule id="{0A58A75E-4698-465A-8593-F06B91A3A900}" type="dataBar">
-            <x14:dataBar minLength="0" gradient="0" maxLength="100">
+          <x14:cfRule type="dataBar" id="{0A58A75E-4698-465A-8593-F06B91A3A900}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
               </x14:cfvo>
@@ -6482,11 +6150,11 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I32 I41:I48</xm:sqref>
+          <xm:sqref>I37:I44 I8:I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule id="{564E9A70-D213-4B59-9E35-13A2D63EE04B}" type="dataBar">
-            <x14:dataBar minLength="0" gradient="0" maxLength="100">
+          <x14:cfRule type="dataBar" id="{564E9A70-D213-4B59-9E35-13A2D63EE04B}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
               </x14:cfvo>
@@ -6497,7 +6165,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I33:I40</xm:sqref>
+          <xm:sqref>I29:I36</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Update the schedule in phase two
</commit_message>
<xml_diff>
--- a/Planning/CAR_Project_ Schedule.xlsx
+++ b/Planning/CAR_Project_ Schedule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Desktop\CarPurchasing\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatma\Desktop\CarPurchasing\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$49</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
     <definedName name="vertex42_copyright" hidden="1">"© 2006-2018 Vertex42 LLC"</definedName>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>WBS</t>
   </si>
@@ -379,6 +379,18 @@
   </si>
   <si>
     <t>Wire frames in SDD</t>
+  </si>
+  <si>
+    <t>Thu 5/09/19</t>
+  </si>
+  <si>
+    <t>2.1.9</t>
+  </si>
+  <si>
+    <t>ERD</t>
+  </si>
+  <si>
+    <t>Tue 5/07/2019</t>
   </si>
 </sst>
 </file>
@@ -680,7 +692,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -798,6 +810,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1128,7 +1146,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -1440,46 +1458,64 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="29" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="29" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="31" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1782,7 +1818,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1846,7 +1882,7 @@
                   <a14:compatExt spid="_x0000_s9262"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E200000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E200000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1896,7 +1932,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1939,7 +1975,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1987,7 +2023,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2001,6 +2037,54 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="7972425" cy="8458200"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 9"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7972425" cy="8610600"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2318,11 +2402,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN55"/>
+  <dimension ref="A1:BN56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="7" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2350,29 +2434,29 @@
       <c r="E1" s="94"/>
       <c r="F1" s="94"/>
       <c r="I1" s="74"/>
-      <c r="K1" s="112" t="s">
+      <c r="K1" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
-      <c r="W1" s="112"/>
-      <c r="X1" s="112"/>
-      <c r="Y1" s="112"/>
-      <c r="Z1" s="112"/>
-      <c r="AA1" s="112"/>
-      <c r="AB1" s="112"/>
-      <c r="AC1" s="112"/>
-      <c r="AD1" s="112"/>
-      <c r="AE1" s="112"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="120"/>
+      <c r="T1" s="120"/>
+      <c r="U1" s="120"/>
+      <c r="V1" s="120"/>
+      <c r="W1" s="120"/>
+      <c r="X1" s="120"/>
+      <c r="Y1" s="120"/>
+      <c r="Z1" s="120"/>
+      <c r="AA1" s="120"/>
+      <c r="AB1" s="120"/>
+      <c r="AC1" s="120"/>
+      <c r="AD1" s="120"/>
+      <c r="AE1" s="120"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
@@ -2417,11 +2501,11 @@
       <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="122">
+      <c r="C4" s="114">
         <v>43582</v>
       </c>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
       <c r="F4" s="108"/>
       <c r="G4" s="59" t="s">
         <v>7</v>
@@ -2431,170 +2515,170 @@
       </c>
       <c r="I4" s="57"/>
       <c r="J4" s="16"/>
-      <c r="K4" s="113" t="str">
+      <c r="K4" s="111" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="114"/>
-      <c r="M4" s="114"/>
-      <c r="N4" s="114"/>
-      <c r="O4" s="114"/>
-      <c r="P4" s="114"/>
-      <c r="Q4" s="115"/>
-      <c r="R4" s="113" t="str">
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="113"/>
+      <c r="R4" s="111" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="114"/>
-      <c r="T4" s="114"/>
-      <c r="U4" s="114"/>
-      <c r="V4" s="114"/>
-      <c r="W4" s="114"/>
-      <c r="X4" s="115"/>
-      <c r="Y4" s="113" t="str">
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="U4" s="112"/>
+      <c r="V4" s="112"/>
+      <c r="W4" s="112"/>
+      <c r="X4" s="113"/>
+      <c r="Y4" s="111" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="114"/>
-      <c r="AA4" s="114"/>
-      <c r="AB4" s="114"/>
-      <c r="AC4" s="114"/>
-      <c r="AD4" s="114"/>
-      <c r="AE4" s="115"/>
-      <c r="AF4" s="113" t="str">
+      <c r="Z4" s="112"/>
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="112"/>
+      <c r="AC4" s="112"/>
+      <c r="AD4" s="112"/>
+      <c r="AE4" s="113"/>
+      <c r="AF4" s="111" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="114"/>
-      <c r="AH4" s="114"/>
-      <c r="AI4" s="114"/>
-      <c r="AJ4" s="114"/>
-      <c r="AK4" s="114"/>
-      <c r="AL4" s="115"/>
-      <c r="AM4" s="113" t="str">
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="112"/>
+      <c r="AI4" s="112"/>
+      <c r="AJ4" s="112"/>
+      <c r="AK4" s="112"/>
+      <c r="AL4" s="113"/>
+      <c r="AM4" s="111" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="114"/>
-      <c r="AO4" s="114"/>
-      <c r="AP4" s="114"/>
-      <c r="AQ4" s="114"/>
-      <c r="AR4" s="114"/>
-      <c r="AS4" s="115"/>
-      <c r="AT4" s="113" t="str">
+      <c r="AN4" s="112"/>
+      <c r="AO4" s="112"/>
+      <c r="AP4" s="112"/>
+      <c r="AQ4" s="112"/>
+      <c r="AR4" s="112"/>
+      <c r="AS4" s="113"/>
+      <c r="AT4" s="111" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="114"/>
-      <c r="AV4" s="114"/>
-      <c r="AW4" s="114"/>
-      <c r="AX4" s="114"/>
-      <c r="AY4" s="114"/>
-      <c r="AZ4" s="119"/>
-      <c r="BA4" s="111"/>
-      <c r="BB4" s="111"/>
-      <c r="BC4" s="111"/>
-      <c r="BD4" s="111"/>
-      <c r="BE4" s="111"/>
-      <c r="BF4" s="111"/>
-      <c r="BG4" s="111"/>
-      <c r="BH4" s="111"/>
-      <c r="BI4" s="111"/>
-      <c r="BJ4" s="111"/>
-      <c r="BK4" s="111"/>
-      <c r="BL4" s="111"/>
-      <c r="BM4" s="111"/>
-      <c r="BN4" s="111"/>
+      <c r="AU4" s="112"/>
+      <c r="AV4" s="112"/>
+      <c r="AW4" s="112"/>
+      <c r="AX4" s="112"/>
+      <c r="AY4" s="112"/>
+      <c r="AZ4" s="121"/>
+      <c r="BA4" s="119"/>
+      <c r="BB4" s="119"/>
+      <c r="BC4" s="119"/>
+      <c r="BD4" s="119"/>
+      <c r="BE4" s="119"/>
+      <c r="BF4" s="119"/>
+      <c r="BG4" s="119"/>
+      <c r="BH4" s="119"/>
+      <c r="BI4" s="119"/>
+      <c r="BJ4" s="119"/>
+      <c r="BK4" s="119"/>
+      <c r="BL4" s="119"/>
+      <c r="BM4" s="119"/>
+      <c r="BN4" s="119"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="56"/>
       <c r="B5" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="121" t="s">
+      <c r="C5" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
       <c r="F5" s="109"/>
       <c r="G5" s="58"/>
       <c r="H5" s="95"/>
       <c r="I5" s="58"/>
       <c r="J5" s="16"/>
-      <c r="K5" s="116">
+      <c r="K5" s="115">
         <f>K6</f>
         <v>43577</v>
       </c>
-      <c r="L5" s="117"/>
-      <c r="M5" s="117"/>
-      <c r="N5" s="117"/>
-      <c r="O5" s="117"/>
-      <c r="P5" s="117"/>
-      <c r="Q5" s="118"/>
-      <c r="R5" s="116">
+      <c r="L5" s="116"/>
+      <c r="M5" s="116"/>
+      <c r="N5" s="116"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="116"/>
+      <c r="Q5" s="117"/>
+      <c r="R5" s="115">
         <f>R6</f>
         <v>43584</v>
       </c>
-      <c r="S5" s="117"/>
-      <c r="T5" s="117"/>
-      <c r="U5" s="117"/>
-      <c r="V5" s="117"/>
-      <c r="W5" s="117"/>
-      <c r="X5" s="118"/>
-      <c r="Y5" s="116">
+      <c r="S5" s="116"/>
+      <c r="T5" s="116"/>
+      <c r="U5" s="116"/>
+      <c r="V5" s="116"/>
+      <c r="W5" s="116"/>
+      <c r="X5" s="117"/>
+      <c r="Y5" s="115">
         <f>Y6</f>
         <v>43591</v>
       </c>
-      <c r="Z5" s="117"/>
-      <c r="AA5" s="117"/>
-      <c r="AB5" s="117"/>
-      <c r="AC5" s="117"/>
-      <c r="AD5" s="117"/>
-      <c r="AE5" s="118"/>
-      <c r="AF5" s="116">
+      <c r="Z5" s="116"/>
+      <c r="AA5" s="116"/>
+      <c r="AB5" s="116"/>
+      <c r="AC5" s="116"/>
+      <c r="AD5" s="116"/>
+      <c r="AE5" s="117"/>
+      <c r="AF5" s="115">
         <f>AF6</f>
         <v>43598</v>
       </c>
-      <c r="AG5" s="117"/>
-      <c r="AH5" s="117"/>
-      <c r="AI5" s="117"/>
-      <c r="AJ5" s="117"/>
-      <c r="AK5" s="117"/>
-      <c r="AL5" s="118"/>
-      <c r="AM5" s="116">
+      <c r="AG5" s="116"/>
+      <c r="AH5" s="116"/>
+      <c r="AI5" s="116"/>
+      <c r="AJ5" s="116"/>
+      <c r="AK5" s="116"/>
+      <c r="AL5" s="117"/>
+      <c r="AM5" s="115">
         <f>AM6</f>
         <v>43605</v>
       </c>
-      <c r="AN5" s="117"/>
-      <c r="AO5" s="117"/>
-      <c r="AP5" s="117"/>
-      <c r="AQ5" s="117"/>
-      <c r="AR5" s="117"/>
-      <c r="AS5" s="118"/>
-      <c r="AT5" s="116">
+      <c r="AN5" s="116"/>
+      <c r="AO5" s="116"/>
+      <c r="AP5" s="116"/>
+      <c r="AQ5" s="116"/>
+      <c r="AR5" s="116"/>
+      <c r="AS5" s="117"/>
+      <c r="AT5" s="115">
         <f>AT6</f>
         <v>43612</v>
       </c>
-      <c r="AU5" s="117"/>
-      <c r="AV5" s="117"/>
-      <c r="AW5" s="117"/>
-      <c r="AX5" s="117"/>
-      <c r="AY5" s="117"/>
-      <c r="AZ5" s="120"/>
-      <c r="BA5" s="110"/>
-      <c r="BB5" s="110"/>
-      <c r="BC5" s="110"/>
-      <c r="BD5" s="110"/>
-      <c r="BE5" s="110"/>
-      <c r="BF5" s="110"/>
-      <c r="BG5" s="110"/>
-      <c r="BH5" s="110"/>
-      <c r="BI5" s="110"/>
-      <c r="BJ5" s="110"/>
-      <c r="BK5" s="110"/>
-      <c r="BL5" s="110"/>
-      <c r="BM5" s="110"/>
-      <c r="BN5" s="110"/>
+      <c r="AU5" s="116"/>
+      <c r="AV5" s="116"/>
+      <c r="AW5" s="116"/>
+      <c r="AX5" s="116"/>
+      <c r="AY5" s="116"/>
+      <c r="AZ5" s="122"/>
+      <c r="BA5" s="118"/>
+      <c r="BB5" s="118"/>
+      <c r="BC5" s="118"/>
+      <c r="BD5" s="118"/>
+      <c r="BE5" s="118"/>
+      <c r="BF5" s="118"/>
+      <c r="BG5" s="118"/>
+      <c r="BH5" s="118"/>
+      <c r="BI5" s="118"/>
+      <c r="BJ5" s="118"/>
+      <c r="BK5" s="118"/>
+      <c r="BL5" s="118"/>
+      <c r="BM5" s="118"/>
+      <c r="BN5" s="118"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="15"/>
@@ -3018,7 +3102,7 @@
       <c r="G8" s="41"/>
       <c r="H8" s="42"/>
       <c r="I8" s="43">
-        <f t="shared" ref="I8:I48" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I49" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v>5</v>
       </c>
       <c r="J8" s="46"/>
@@ -4011,8 +4095,8 @@
       <c r="R20" s="53"/>
       <c r="S20" s="53"/>
       <c r="T20" s="53"/>
-      <c r="U20" s="53"/>
-      <c r="V20" s="53"/>
+      <c r="U20" s="123"/>
+      <c r="V20" s="123"/>
       <c r="W20" s="53"/>
       <c r="X20" s="53"/>
       <c r="Y20" s="53"/>
@@ -4069,15 +4153,20 @@
         <v>51</v>
       </c>
       <c r="D21" s="72"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="98"/>
-      <c r="G21" s="28"/>
+      <c r="E21" s="98" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="28">
+        <v>1</v>
+      </c>
       <c r="H21" s="29">
-        <v>0</v>
-      </c>
-      <c r="I21" s="30" t="str">
-        <f>IF(OR(F19=0,E21=0)," - ",NETWORKDAYS(E21,F19))</f>
-        <v xml:space="preserve"> - </v>
+        <v>1</v>
+      </c>
+      <c r="I21" s="30">
+        <v>2</v>
       </c>
       <c r="J21" s="47"/>
       <c r="K21" s="53"/>
@@ -4517,157 +4606,169 @@
       <c r="BM26" s="53"/>
       <c r="BN26" s="53"/>
     </row>
-    <row r="27" spans="1:66" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="19"/>
-      <c r="B27" s="20" t="s">
+    <row r="27" spans="1:66" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="86" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="124"/>
+      <c r="E27" s="125" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="125" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="126">
+        <v>1</v>
+      </c>
+      <c r="H27" s="29">
+        <v>1</v>
+      </c>
+      <c r="I27" s="127">
+        <v>1</v>
+      </c>
+      <c r="J27" s="128"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="123"/>
+      <c r="T27" s="53"/>
+      <c r="U27" s="53"/>
+      <c r="V27" s="53"/>
+      <c r="W27" s="53"/>
+      <c r="X27" s="53"/>
+      <c r="Y27" s="53"/>
+      <c r="Z27" s="53"/>
+      <c r="AA27" s="53"/>
+      <c r="AB27" s="53"/>
+      <c r="AC27" s="53"/>
+      <c r="AD27" s="53"/>
+      <c r="AE27" s="53"/>
+      <c r="AF27" s="53"/>
+      <c r="AG27" s="53"/>
+      <c r="AH27" s="53"/>
+      <c r="AI27" s="53"/>
+      <c r="AJ27" s="53"/>
+      <c r="AK27" s="53"/>
+      <c r="AL27" s="53"/>
+      <c r="AM27" s="53"/>
+      <c r="AN27" s="53"/>
+      <c r="AO27" s="53"/>
+      <c r="AP27" s="53"/>
+      <c r="AQ27" s="53"/>
+      <c r="AR27" s="53"/>
+      <c r="AS27" s="53"/>
+      <c r="AT27" s="53"/>
+      <c r="AU27" s="53"/>
+      <c r="AV27" s="53"/>
+      <c r="AW27" s="53"/>
+      <c r="AX27" s="53"/>
+      <c r="AY27" s="53"/>
+      <c r="AZ27" s="53"/>
+      <c r="BA27" s="53"/>
+      <c r="BB27" s="53"/>
+      <c r="BC27" s="53"/>
+      <c r="BD27" s="53"/>
+      <c r="BE27" s="53"/>
+      <c r="BF27" s="53"/>
+      <c r="BG27" s="53"/>
+      <c r="BH27" s="53"/>
+      <c r="BI27" s="53"/>
+      <c r="BJ27" s="53"/>
+      <c r="BK27" s="53"/>
+      <c r="BL27" s="53"/>
+      <c r="BM27" s="53"/>
+      <c r="BN27" s="53"/>
+    </row>
+    <row r="28" spans="1:66" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="25" t="str">
+      <c r="D28" s="22"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="25" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J27" s="48"/>
-      <c r="K27" s="55"/>
-      <c r="L27" s="55"/>
-      <c r="M27" s="55"/>
-      <c r="N27" s="55"/>
-      <c r="O27" s="55"/>
-      <c r="P27" s="55"/>
-      <c r="Q27" s="55"/>
-      <c r="R27" s="55"/>
-      <c r="S27" s="55"/>
-      <c r="T27" s="55"/>
-      <c r="U27" s="55"/>
-      <c r="V27" s="55"/>
-      <c r="W27" s="55"/>
-      <c r="X27" s="55"/>
-      <c r="Y27" s="55"/>
-      <c r="Z27" s="55"/>
-      <c r="AA27" s="55"/>
-      <c r="AB27" s="55"/>
-      <c r="AC27" s="55"/>
-      <c r="AD27" s="55"/>
-      <c r="AE27" s="55"/>
-      <c r="AF27" s="55"/>
-      <c r="AG27" s="55"/>
-      <c r="AH27" s="55"/>
-      <c r="AI27" s="55"/>
-      <c r="AJ27" s="55"/>
-      <c r="AK27" s="55"/>
-      <c r="AL27" s="55"/>
-      <c r="AM27" s="55"/>
-      <c r="AN27" s="55"/>
-      <c r="AO27" s="55"/>
-      <c r="AP27" s="55"/>
-      <c r="AQ27" s="55"/>
-      <c r="AR27" s="55"/>
-      <c r="AS27" s="55"/>
-      <c r="AT27" s="55"/>
-      <c r="AU27" s="55"/>
-      <c r="AV27" s="55"/>
-      <c r="AW27" s="55"/>
-      <c r="AX27" s="55"/>
-      <c r="AY27" s="55"/>
-      <c r="AZ27" s="55"/>
-      <c r="BA27" s="55"/>
-      <c r="BB27" s="55"/>
-      <c r="BC27" s="55"/>
-      <c r="BD27" s="55"/>
-      <c r="BE27" s="55"/>
-      <c r="BF27" s="55"/>
-      <c r="BG27" s="55"/>
-      <c r="BH27" s="55"/>
-      <c r="BI27" s="55"/>
-      <c r="BJ27" s="55"/>
-      <c r="BK27" s="55"/>
-      <c r="BL27" s="55"/>
-      <c r="BM27" s="55"/>
-      <c r="BN27" s="55"/>
-    </row>
-    <row r="28" spans="1:66" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A28" s="26">
-        <v>3.1</v>
-      </c>
-      <c r="B28" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="72"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="29">
-        <v>0</v>
-      </c>
-      <c r="I28" s="30" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J28" s="47"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="53"/>
-      <c r="N28" s="53"/>
-      <c r="O28" s="53"/>
-      <c r="P28" s="53"/>
-      <c r="Q28" s="53"/>
-      <c r="R28" s="53"/>
-      <c r="S28" s="53"/>
-      <c r="T28" s="53"/>
-      <c r="U28" s="53"/>
-      <c r="V28" s="53"/>
-      <c r="W28" s="53"/>
-      <c r="X28" s="53"/>
-      <c r="Y28" s="53"/>
-      <c r="Z28" s="53"/>
-      <c r="AA28" s="53"/>
-      <c r="AB28" s="53"/>
-      <c r="AC28" s="53"/>
-      <c r="AD28" s="53"/>
-      <c r="AE28" s="53"/>
-      <c r="AF28" s="53"/>
-      <c r="AG28" s="53"/>
-      <c r="AH28" s="53"/>
-      <c r="AI28" s="53"/>
-      <c r="AJ28" s="53"/>
-      <c r="AK28" s="53"/>
-      <c r="AL28" s="53"/>
-      <c r="AM28" s="53"/>
-      <c r="AN28" s="53"/>
-      <c r="AO28" s="53"/>
-      <c r="AP28" s="53"/>
-      <c r="AQ28" s="53"/>
-      <c r="AR28" s="53"/>
-      <c r="AS28" s="53"/>
-      <c r="AT28" s="53"/>
-      <c r="AU28" s="53"/>
-      <c r="AV28" s="53"/>
-      <c r="AW28" s="53"/>
-      <c r="AX28" s="53"/>
-      <c r="AY28" s="53"/>
-      <c r="AZ28" s="53"/>
-      <c r="BA28" s="53"/>
-      <c r="BB28" s="53"/>
-      <c r="BC28" s="53"/>
-      <c r="BD28" s="53"/>
-      <c r="BE28" s="53"/>
-      <c r="BF28" s="53"/>
-      <c r="BG28" s="53"/>
-      <c r="BH28" s="53"/>
-      <c r="BI28" s="53"/>
-      <c r="BJ28" s="53"/>
-      <c r="BK28" s="53"/>
-      <c r="BL28" s="53"/>
-      <c r="BM28" s="53"/>
-      <c r="BN28" s="53"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="55"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="55"/>
+      <c r="T28" s="55"/>
+      <c r="U28" s="55"/>
+      <c r="V28" s="55"/>
+      <c r="W28" s="55"/>
+      <c r="X28" s="55"/>
+      <c r="Y28" s="55"/>
+      <c r="Z28" s="55"/>
+      <c r="AA28" s="55"/>
+      <c r="AB28" s="55"/>
+      <c r="AC28" s="55"/>
+      <c r="AD28" s="55"/>
+      <c r="AE28" s="55"/>
+      <c r="AF28" s="55"/>
+      <c r="AG28" s="55"/>
+      <c r="AH28" s="55"/>
+      <c r="AI28" s="55"/>
+      <c r="AJ28" s="55"/>
+      <c r="AK28" s="55"/>
+      <c r="AL28" s="55"/>
+      <c r="AM28" s="55"/>
+      <c r="AN28" s="55"/>
+      <c r="AO28" s="55"/>
+      <c r="AP28" s="55"/>
+      <c r="AQ28" s="55"/>
+      <c r="AR28" s="55"/>
+      <c r="AS28" s="55"/>
+      <c r="AT28" s="55"/>
+      <c r="AU28" s="55"/>
+      <c r="AV28" s="55"/>
+      <c r="AW28" s="55"/>
+      <c r="AX28" s="55"/>
+      <c r="AY28" s="55"/>
+      <c r="AZ28" s="55"/>
+      <c r="BA28" s="55"/>
+      <c r="BB28" s="55"/>
+      <c r="BC28" s="55"/>
+      <c r="BD28" s="55"/>
+      <c r="BE28" s="55"/>
+      <c r="BF28" s="55"/>
+      <c r="BG28" s="55"/>
+      <c r="BH28" s="55"/>
+      <c r="BI28" s="55"/>
+      <c r="BJ28" s="55"/>
+      <c r="BK28" s="55"/>
+      <c r="BL28" s="55"/>
+      <c r="BM28" s="55"/>
+      <c r="BN28" s="55"/>
     </row>
     <row r="29" spans="1:66" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="26"/>
-      <c r="B29" s="71"/>
+      <c r="A29" s="26">
+        <v>3.1</v>
+      </c>
+      <c r="B29" s="71" t="s">
+        <v>36</v>
+      </c>
       <c r="D29" s="72"/>
       <c r="E29" s="98"/>
       <c r="F29" s="50"/>
@@ -4953,157 +5054,157 @@
       <c r="BM32" s="53"/>
       <c r="BN32" s="53"/>
     </row>
-    <row r="33" spans="1:66" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20" t="s">
+    <row r="33" spans="1:66" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="26"/>
+      <c r="B33" s="71"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="29">
+        <v>0</v>
+      </c>
+      <c r="I33" s="30" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J33" s="47"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="53"/>
+      <c r="N33" s="53"/>
+      <c r="O33" s="53"/>
+      <c r="P33" s="53"/>
+      <c r="Q33" s="53"/>
+      <c r="R33" s="53"/>
+      <c r="S33" s="53"/>
+      <c r="T33" s="53"/>
+      <c r="U33" s="53"/>
+      <c r="V33" s="53"/>
+      <c r="W33" s="53"/>
+      <c r="X33" s="53"/>
+      <c r="Y33" s="53"/>
+      <c r="Z33" s="53"/>
+      <c r="AA33" s="53"/>
+      <c r="AB33" s="53"/>
+      <c r="AC33" s="53"/>
+      <c r="AD33" s="53"/>
+      <c r="AE33" s="53"/>
+      <c r="AF33" s="53"/>
+      <c r="AG33" s="53"/>
+      <c r="AH33" s="53"/>
+      <c r="AI33" s="53"/>
+      <c r="AJ33" s="53"/>
+      <c r="AK33" s="53"/>
+      <c r="AL33" s="53"/>
+      <c r="AM33" s="53"/>
+      <c r="AN33" s="53"/>
+      <c r="AO33" s="53"/>
+      <c r="AP33" s="53"/>
+      <c r="AQ33" s="53"/>
+      <c r="AR33" s="53"/>
+      <c r="AS33" s="53"/>
+      <c r="AT33" s="53"/>
+      <c r="AU33" s="53"/>
+      <c r="AV33" s="53"/>
+      <c r="AW33" s="53"/>
+      <c r="AX33" s="53"/>
+      <c r="AY33" s="53"/>
+      <c r="AZ33" s="53"/>
+      <c r="BA33" s="53"/>
+      <c r="BB33" s="53"/>
+      <c r="BC33" s="53"/>
+      <c r="BD33" s="53"/>
+      <c r="BE33" s="53"/>
+      <c r="BF33" s="53"/>
+      <c r="BG33" s="53"/>
+      <c r="BH33" s="53"/>
+      <c r="BI33" s="53"/>
+      <c r="BJ33" s="53"/>
+      <c r="BK33" s="53"/>
+      <c r="BL33" s="53"/>
+      <c r="BM33" s="53"/>
+      <c r="BN33" s="53"/>
+    </row>
+    <row r="34" spans="1:66" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="19"/>
+      <c r="B34" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="25" t="str">
-        <f t="shared" ref="I33:I40" si="5">IF(OR(F33=0,E33=0)," - ",NETWORKDAYS(E33,F33))</f>
+      <c r="D34" s="22"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="25" t="str">
+        <f t="shared" ref="I34:I41" si="5">IF(OR(F34=0,E34=0)," - ",NETWORKDAYS(E34,F34))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J33" s="48"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="55"/>
-      <c r="M33" s="55"/>
-      <c r="N33" s="55"/>
-      <c r="O33" s="55"/>
-      <c r="P33" s="55"/>
-      <c r="Q33" s="55"/>
-      <c r="R33" s="55"/>
-      <c r="S33" s="55"/>
-      <c r="T33" s="55"/>
-      <c r="U33" s="55"/>
-      <c r="V33" s="55"/>
-      <c r="W33" s="55"/>
-      <c r="X33" s="55"/>
-      <c r="Y33" s="55"/>
-      <c r="Z33" s="55"/>
-      <c r="AA33" s="55"/>
-      <c r="AB33" s="55"/>
-      <c r="AC33" s="55"/>
-      <c r="AD33" s="55"/>
-      <c r="AE33" s="55"/>
-      <c r="AF33" s="55"/>
-      <c r="AG33" s="55"/>
-      <c r="AH33" s="55"/>
-      <c r="AI33" s="55"/>
-      <c r="AJ33" s="55"/>
-      <c r="AK33" s="55"/>
-      <c r="AL33" s="55"/>
-      <c r="AM33" s="55"/>
-      <c r="AN33" s="55"/>
-      <c r="AO33" s="55"/>
-      <c r="AP33" s="55"/>
-      <c r="AQ33" s="55"/>
-      <c r="AR33" s="55"/>
-      <c r="AS33" s="55"/>
-      <c r="AT33" s="55"/>
-      <c r="AU33" s="55"/>
-      <c r="AV33" s="55"/>
-      <c r="AW33" s="55"/>
-      <c r="AX33" s="55"/>
-      <c r="AY33" s="55"/>
-      <c r="AZ33" s="55"/>
-      <c r="BA33" s="55"/>
-      <c r="BB33" s="55"/>
-      <c r="BC33" s="55"/>
-      <c r="BD33" s="55"/>
-      <c r="BE33" s="55"/>
-      <c r="BF33" s="55"/>
-      <c r="BG33" s="55"/>
-      <c r="BH33" s="55"/>
-      <c r="BI33" s="55"/>
-      <c r="BJ33" s="55"/>
-      <c r="BK33" s="55"/>
-      <c r="BL33" s="55"/>
-      <c r="BM33" s="55"/>
-      <c r="BN33" s="55"/>
-    </row>
-    <row r="34" spans="1:66" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="26">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B34" s="71" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="72"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="29">
-        <v>0</v>
-      </c>
-      <c r="I34" s="30" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J34" s="47"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="53"/>
-      <c r="M34" s="53"/>
-      <c r="N34" s="53"/>
-      <c r="O34" s="53"/>
-      <c r="P34" s="53"/>
-      <c r="Q34" s="53"/>
-      <c r="R34" s="53"/>
-      <c r="S34" s="53"/>
-      <c r="T34" s="53"/>
-      <c r="U34" s="53"/>
-      <c r="V34" s="53"/>
-      <c r="W34" s="53"/>
-      <c r="X34" s="53"/>
-      <c r="Y34" s="53"/>
-      <c r="Z34" s="53"/>
-      <c r="AA34" s="53"/>
-      <c r="AB34" s="53"/>
-      <c r="AC34" s="53"/>
-      <c r="AD34" s="53"/>
-      <c r="AE34" s="53"/>
-      <c r="AF34" s="53"/>
-      <c r="AG34" s="53"/>
-      <c r="AH34" s="53"/>
-      <c r="AI34" s="53"/>
-      <c r="AJ34" s="53"/>
-      <c r="AK34" s="53"/>
-      <c r="AL34" s="53"/>
-      <c r="AM34" s="53"/>
-      <c r="AN34" s="53"/>
-      <c r="AO34" s="53"/>
-      <c r="AP34" s="53"/>
-      <c r="AQ34" s="53"/>
-      <c r="AR34" s="53"/>
-      <c r="AS34" s="53"/>
-      <c r="AT34" s="53"/>
-      <c r="AU34" s="53"/>
-      <c r="AV34" s="53"/>
-      <c r="AW34" s="53"/>
-      <c r="AX34" s="53"/>
-      <c r="AY34" s="53"/>
-      <c r="AZ34" s="53"/>
-      <c r="BA34" s="53"/>
-      <c r="BB34" s="53"/>
-      <c r="BC34" s="53"/>
-      <c r="BD34" s="53"/>
-      <c r="BE34" s="53"/>
-      <c r="BF34" s="53"/>
-      <c r="BG34" s="53"/>
-      <c r="BH34" s="53"/>
-      <c r="BI34" s="53"/>
-      <c r="BJ34" s="53"/>
-      <c r="BK34" s="53"/>
-      <c r="BL34" s="53"/>
-      <c r="BM34" s="53"/>
-      <c r="BN34" s="53"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="55"/>
+      <c r="N34" s="55"/>
+      <c r="O34" s="55"/>
+      <c r="P34" s="55"/>
+      <c r="Q34" s="55"/>
+      <c r="R34" s="55"/>
+      <c r="S34" s="55"/>
+      <c r="T34" s="55"/>
+      <c r="U34" s="55"/>
+      <c r="V34" s="55"/>
+      <c r="W34" s="55"/>
+      <c r="X34" s="55"/>
+      <c r="Y34" s="55"/>
+      <c r="Z34" s="55"/>
+      <c r="AA34" s="55"/>
+      <c r="AB34" s="55"/>
+      <c r="AC34" s="55"/>
+      <c r="AD34" s="55"/>
+      <c r="AE34" s="55"/>
+      <c r="AF34" s="55"/>
+      <c r="AG34" s="55"/>
+      <c r="AH34" s="55"/>
+      <c r="AI34" s="55"/>
+      <c r="AJ34" s="55"/>
+      <c r="AK34" s="55"/>
+      <c r="AL34" s="55"/>
+      <c r="AM34" s="55"/>
+      <c r="AN34" s="55"/>
+      <c r="AO34" s="55"/>
+      <c r="AP34" s="55"/>
+      <c r="AQ34" s="55"/>
+      <c r="AR34" s="55"/>
+      <c r="AS34" s="55"/>
+      <c r="AT34" s="55"/>
+      <c r="AU34" s="55"/>
+      <c r="AV34" s="55"/>
+      <c r="AW34" s="55"/>
+      <c r="AX34" s="55"/>
+      <c r="AY34" s="55"/>
+      <c r="AZ34" s="55"/>
+      <c r="BA34" s="55"/>
+      <c r="BB34" s="55"/>
+      <c r="BC34" s="55"/>
+      <c r="BD34" s="55"/>
+      <c r="BE34" s="55"/>
+      <c r="BF34" s="55"/>
+      <c r="BG34" s="55"/>
+      <c r="BH34" s="55"/>
+      <c r="BI34" s="55"/>
+      <c r="BJ34" s="55"/>
+      <c r="BK34" s="55"/>
+      <c r="BL34" s="55"/>
+      <c r="BM34" s="55"/>
+      <c r="BN34" s="55"/>
     </row>
     <row r="35" spans="1:66" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="26"/>
-      <c r="B35" s="71"/>
+      <c r="A35" s="26">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B35" s="71" t="s">
+        <v>38</v>
+      </c>
       <c r="D35" s="72"/>
       <c r="E35" s="98"/>
       <c r="F35" s="50"/>
@@ -5321,10 +5422,10 @@
       <c r="A38" s="26"/>
       <c r="B38" s="71"/>
       <c r="D38" s="72"/>
-      <c r="E38" s="105"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="88"/>
-      <c r="H38" s="89">
+      <c r="E38" s="98"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="29">
         <v>0</v>
       </c>
       <c r="I38" s="30" t="str">
@@ -5389,20 +5490,21 @@
       <c r="BM38" s="53"/>
       <c r="BN38" s="53"/>
     </row>
-    <row r="39" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:66" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="26"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="90"/>
-      <c r="F39" s="90"/>
-      <c r="G39" s="91"/>
-      <c r="H39" s="92"/>
-      <c r="I39" s="33" t="str">
+      <c r="B39" s="71"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="105"/>
+      <c r="F39" s="87"/>
+      <c r="G39" s="88"/>
+      <c r="H39" s="89">
+        <v>0</v>
+      </c>
+      <c r="I39" s="30" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J39" s="49"/>
+      <c r="J39" s="47"/>
       <c r="K39" s="53"/>
       <c r="L39" s="53"/>
       <c r="M39" s="53"/>
@@ -5531,157 +5633,156 @@
       <c r="BM40" s="53"/>
       <c r="BN40" s="53"/>
     </row>
-    <row r="41" spans="1:66" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A41" s="19"/>
-      <c r="B41" s="20" t="s">
+    <row r="41" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="26"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="90"/>
+      <c r="G41" s="91"/>
+      <c r="H41" s="92"/>
+      <c r="I41" s="33" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J41" s="49"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="53"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="53"/>
+      <c r="R41" s="53"/>
+      <c r="S41" s="53"/>
+      <c r="T41" s="53"/>
+      <c r="U41" s="53"/>
+      <c r="V41" s="53"/>
+      <c r="W41" s="53"/>
+      <c r="X41" s="53"/>
+      <c r="Y41" s="53"/>
+      <c r="Z41" s="53"/>
+      <c r="AA41" s="53"/>
+      <c r="AB41" s="53"/>
+      <c r="AC41" s="53"/>
+      <c r="AD41" s="53"/>
+      <c r="AE41" s="53"/>
+      <c r="AF41" s="53"/>
+      <c r="AG41" s="53"/>
+      <c r="AH41" s="53"/>
+      <c r="AI41" s="53"/>
+      <c r="AJ41" s="53"/>
+      <c r="AK41" s="53"/>
+      <c r="AL41" s="53"/>
+      <c r="AM41" s="53"/>
+      <c r="AN41" s="53"/>
+      <c r="AO41" s="53"/>
+      <c r="AP41" s="53"/>
+      <c r="AQ41" s="53"/>
+      <c r="AR41" s="53"/>
+      <c r="AS41" s="53"/>
+      <c r="AT41" s="53"/>
+      <c r="AU41" s="53"/>
+      <c r="AV41" s="53"/>
+      <c r="AW41" s="53"/>
+      <c r="AX41" s="53"/>
+      <c r="AY41" s="53"/>
+      <c r="AZ41" s="53"/>
+      <c r="BA41" s="53"/>
+      <c r="BB41" s="53"/>
+      <c r="BC41" s="53"/>
+      <c r="BD41" s="53"/>
+      <c r="BE41" s="53"/>
+      <c r="BF41" s="53"/>
+      <c r="BG41" s="53"/>
+      <c r="BH41" s="53"/>
+      <c r="BI41" s="53"/>
+      <c r="BJ41" s="53"/>
+      <c r="BK41" s="53"/>
+      <c r="BL41" s="53"/>
+      <c r="BM41" s="53"/>
+      <c r="BN41" s="53"/>
+    </row>
+    <row r="42" spans="1:66" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="19"/>
+      <c r="B42" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="25" t="str">
+      <c r="D42" s="22"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="25" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J41" s="48"/>
-      <c r="K41" s="55"/>
-      <c r="L41" s="55"/>
-      <c r="M41" s="55"/>
-      <c r="N41" s="55"/>
-      <c r="O41" s="55"/>
-      <c r="P41" s="55"/>
-      <c r="Q41" s="55"/>
-      <c r="R41" s="55"/>
-      <c r="S41" s="55"/>
-      <c r="T41" s="55"/>
-      <c r="U41" s="55"/>
-      <c r="V41" s="55"/>
-      <c r="W41" s="55"/>
-      <c r="X41" s="55"/>
-      <c r="Y41" s="55"/>
-      <c r="Z41" s="55"/>
-      <c r="AA41" s="55"/>
-      <c r="AB41" s="55"/>
-      <c r="AC41" s="55"/>
-      <c r="AD41" s="55"/>
-      <c r="AE41" s="55"/>
-      <c r="AF41" s="55"/>
-      <c r="AG41" s="55"/>
-      <c r="AH41" s="55"/>
-      <c r="AI41" s="55"/>
-      <c r="AJ41" s="55"/>
-      <c r="AK41" s="55"/>
-      <c r="AL41" s="55"/>
-      <c r="AM41" s="55"/>
-      <c r="AN41" s="55"/>
-      <c r="AO41" s="55"/>
-      <c r="AP41" s="55"/>
-      <c r="AQ41" s="55"/>
-      <c r="AR41" s="55"/>
-      <c r="AS41" s="55"/>
-      <c r="AT41" s="55"/>
-      <c r="AU41" s="55"/>
-      <c r="AV41" s="55"/>
-      <c r="AW41" s="55"/>
-      <c r="AX41" s="55"/>
-      <c r="AY41" s="55"/>
-      <c r="AZ41" s="55"/>
-      <c r="BA41" s="55"/>
-      <c r="BB41" s="55"/>
-      <c r="BC41" s="55"/>
-      <c r="BD41" s="55"/>
-      <c r="BE41" s="55"/>
-      <c r="BF41" s="55"/>
-      <c r="BG41" s="55"/>
-      <c r="BH41" s="55"/>
-      <c r="BI41" s="55"/>
-      <c r="BJ41" s="55"/>
-      <c r="BK41" s="55"/>
-      <c r="BL41" s="55"/>
-      <c r="BM41" s="55"/>
-      <c r="BN41" s="55"/>
-    </row>
-    <row r="42" spans="1:66" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A42" s="26">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B42" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="D42" s="72"/>
-      <c r="E42" s="98"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="29">
-        <v>0</v>
-      </c>
-      <c r="I42" s="30" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J42" s="47"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="53"/>
-      <c r="M42" s="53"/>
-      <c r="N42" s="53"/>
-      <c r="O42" s="53"/>
-      <c r="P42" s="53"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="53"/>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
-      <c r="U42" s="53"/>
-      <c r="V42" s="53"/>
-      <c r="W42" s="53"/>
-      <c r="X42" s="53"/>
-      <c r="Y42" s="53"/>
-      <c r="Z42" s="53"/>
-      <c r="AA42" s="53"/>
-      <c r="AB42" s="53"/>
-      <c r="AC42" s="53"/>
-      <c r="AD42" s="53"/>
-      <c r="AE42" s="53"/>
-      <c r="AF42" s="53"/>
-      <c r="AG42" s="53"/>
-      <c r="AH42" s="53"/>
-      <c r="AI42" s="53"/>
-      <c r="AJ42" s="53"/>
-      <c r="AK42" s="53"/>
-      <c r="AL42" s="53"/>
-      <c r="AM42" s="53"/>
-      <c r="AN42" s="53"/>
-      <c r="AO42" s="53"/>
-      <c r="AP42" s="53"/>
-      <c r="AQ42" s="53"/>
-      <c r="AR42" s="53"/>
-      <c r="AS42" s="53"/>
-      <c r="AT42" s="53"/>
-      <c r="AU42" s="53"/>
-      <c r="AV42" s="53"/>
-      <c r="AW42" s="53"/>
-      <c r="AX42" s="53"/>
-      <c r="AY42" s="53"/>
-      <c r="AZ42" s="53"/>
-      <c r="BA42" s="53"/>
-      <c r="BB42" s="53"/>
-      <c r="BC42" s="53"/>
-      <c r="BD42" s="53"/>
-      <c r="BE42" s="53"/>
-      <c r="BF42" s="53"/>
-      <c r="BG42" s="53"/>
-      <c r="BH42" s="53"/>
-      <c r="BI42" s="53"/>
-      <c r="BJ42" s="53"/>
-      <c r="BK42" s="53"/>
-      <c r="BL42" s="53"/>
-      <c r="BM42" s="53"/>
-      <c r="BN42" s="53"/>
+      <c r="J42" s="48"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="55"/>
+      <c r="M42" s="55"/>
+      <c r="N42" s="55"/>
+      <c r="O42" s="55"/>
+      <c r="P42" s="55"/>
+      <c r="Q42" s="55"/>
+      <c r="R42" s="55"/>
+      <c r="S42" s="55"/>
+      <c r="T42" s="55"/>
+      <c r="U42" s="55"/>
+      <c r="V42" s="55"/>
+      <c r="W42" s="55"/>
+      <c r="X42" s="55"/>
+      <c r="Y42" s="55"/>
+      <c r="Z42" s="55"/>
+      <c r="AA42" s="55"/>
+      <c r="AB42" s="55"/>
+      <c r="AC42" s="55"/>
+      <c r="AD42" s="55"/>
+      <c r="AE42" s="55"/>
+      <c r="AF42" s="55"/>
+      <c r="AG42" s="55"/>
+      <c r="AH42" s="55"/>
+      <c r="AI42" s="55"/>
+      <c r="AJ42" s="55"/>
+      <c r="AK42" s="55"/>
+      <c r="AL42" s="55"/>
+      <c r="AM42" s="55"/>
+      <c r="AN42" s="55"/>
+      <c r="AO42" s="55"/>
+      <c r="AP42" s="55"/>
+      <c r="AQ42" s="55"/>
+      <c r="AR42" s="55"/>
+      <c r="AS42" s="55"/>
+      <c r="AT42" s="55"/>
+      <c r="AU42" s="55"/>
+      <c r="AV42" s="55"/>
+      <c r="AW42" s="55"/>
+      <c r="AX42" s="55"/>
+      <c r="AY42" s="55"/>
+      <c r="AZ42" s="55"/>
+      <c r="BA42" s="55"/>
+      <c r="BB42" s="55"/>
+      <c r="BC42" s="55"/>
+      <c r="BD42" s="55"/>
+      <c r="BE42" s="55"/>
+      <c r="BF42" s="55"/>
+      <c r="BG42" s="55"/>
+      <c r="BH42" s="55"/>
+      <c r="BI42" s="55"/>
+      <c r="BJ42" s="55"/>
+      <c r="BK42" s="55"/>
+      <c r="BL42" s="55"/>
+      <c r="BM42" s="55"/>
+      <c r="BN42" s="55"/>
     </row>
     <row r="43" spans="1:66" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A43" s="26"/>
-      <c r="B43" s="71"/>
+      <c r="A43" s="26">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B43" s="71" t="s">
+        <v>40</v>
+      </c>
       <c r="D43" s="72"/>
       <c r="E43" s="98"/>
       <c r="F43" s="50"/>
@@ -5967,20 +6068,21 @@
       <c r="BM46" s="53"/>
       <c r="BN46" s="53"/>
     </row>
-    <row r="47" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:66" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="26"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="76"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="33" t="str">
+      <c r="B47" s="71"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="98"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="29">
+        <v>0</v>
+      </c>
+      <c r="I47" s="30" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J47" s="49"/>
+      <c r="J47" s="47"/>
       <c r="K47" s="53"/>
       <c r="L47" s="53"/>
       <c r="M47" s="53"/>
@@ -6109,17 +6211,20 @@
       <c r="BM48" s="53"/>
       <c r="BN48" s="53"/>
     </row>
-    <row r="49" spans="1:66" s="35" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A49" s="53"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="93"/>
-      <c r="F49" s="93"/>
-      <c r="G49" s="53"/>
-      <c r="H49" s="93"/>
-      <c r="I49" s="53"/>
-      <c r="J49" s="53"/>
+    <row r="49" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="26"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="76"/>
+      <c r="H49" s="77"/>
+      <c r="I49" s="33" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J49" s="49"/>
       <c r="K49" s="53"/>
       <c r="L49" s="53"/>
       <c r="M49" s="53"/>
@@ -6164,8 +6269,20 @@
       <c r="AZ49" s="53"/>
       <c r="BA49" s="53"/>
       <c r="BB49" s="53"/>
+      <c r="BC49" s="53"/>
+      <c r="BD49" s="53"/>
+      <c r="BE49" s="53"/>
+      <c r="BF49" s="53"/>
+      <c r="BG49" s="53"/>
+      <c r="BH49" s="53"/>
+      <c r="BI49" s="53"/>
+      <c r="BJ49" s="53"/>
+      <c r="BK49" s="53"/>
+      <c r="BL49" s="53"/>
+      <c r="BM49" s="53"/>
+      <c r="BN49" s="53"/>
     </row>
-    <row r="50" spans="1:66" s="34" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:66" s="35" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A50" s="53"/>
       <c r="B50" s="53"/>
       <c r="C50" s="53"/>
@@ -6445,83 +6562,133 @@
       <c r="BA54" s="53"/>
       <c r="BB54" s="53"/>
     </row>
-    <row r="55" spans="1:66" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="8"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="106"/>
-      <c r="F55" s="106"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="99"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
-      <c r="L55" s="9"/>
-      <c r="M55" s="9"/>
-      <c r="N55" s="9"/>
-      <c r="O55" s="9"/>
-      <c r="P55" s="9"/>
-      <c r="Q55" s="9"/>
-      <c r="R55" s="9"/>
-      <c r="S55" s="9"/>
-      <c r="T55" s="9"/>
-      <c r="U55" s="9"/>
-      <c r="V55" s="9"/>
-      <c r="W55" s="9"/>
-      <c r="X55" s="9"/>
-      <c r="Y55" s="9"/>
-      <c r="Z55" s="9"/>
-      <c r="AA55" s="9"/>
-      <c r="AB55" s="9"/>
-      <c r="AC55" s="9"/>
-      <c r="AD55" s="9"/>
-      <c r="AE55" s="9"/>
-      <c r="AF55" s="9"/>
-      <c r="AG55" s="9"/>
-      <c r="AH55" s="9"/>
-      <c r="AI55" s="9"/>
-      <c r="AJ55" s="9"/>
-      <c r="AK55" s="9"/>
-      <c r="AL55" s="9"/>
-      <c r="AM55" s="9"/>
-      <c r="AN55" s="9"/>
-      <c r="AO55" s="9"/>
-      <c r="AP55" s="9"/>
-      <c r="AQ55" s="9"/>
-      <c r="AR55" s="9"/>
-      <c r="AS55" s="9"/>
-      <c r="AT55" s="9"/>
-      <c r="AU55" s="9"/>
-      <c r="AV55" s="9"/>
-      <c r="AW55" s="9"/>
-      <c r="AX55" s="9"/>
-      <c r="AY55" s="9"/>
-      <c r="AZ55" s="9"/>
-      <c r="BA55" s="9"/>
-      <c r="BB55" s="9"/>
-      <c r="BC55" s="9"/>
-      <c r="BD55" s="9"/>
-      <c r="BE55" s="9"/>
-      <c r="BF55" s="9"/>
-      <c r="BG55" s="9"/>
-      <c r="BH55" s="9"/>
-      <c r="BI55" s="9"/>
-      <c r="BJ55" s="9"/>
-      <c r="BK55" s="9"/>
-      <c r="BL55" s="9"/>
-      <c r="BM55" s="9"/>
-      <c r="BN55" s="9"/>
+    <row r="55" spans="1:66" s="34" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A55" s="53"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="93"/>
+      <c r="F55" s="93"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="93"/>
+      <c r="I55" s="53"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="53"/>
+      <c r="L55" s="53"/>
+      <c r="M55" s="53"/>
+      <c r="N55" s="53"/>
+      <c r="O55" s="53"/>
+      <c r="P55" s="53"/>
+      <c r="Q55" s="53"/>
+      <c r="R55" s="53"/>
+      <c r="S55" s="53"/>
+      <c r="T55" s="53"/>
+      <c r="U55" s="53"/>
+      <c r="V55" s="53"/>
+      <c r="W55" s="53"/>
+      <c r="X55" s="53"/>
+      <c r="Y55" s="53"/>
+      <c r="Z55" s="53"/>
+      <c r="AA55" s="53"/>
+      <c r="AB55" s="53"/>
+      <c r="AC55" s="53"/>
+      <c r="AD55" s="53"/>
+      <c r="AE55" s="53"/>
+      <c r="AF55" s="53"/>
+      <c r="AG55" s="53"/>
+      <c r="AH55" s="53"/>
+      <c r="AI55" s="53"/>
+      <c r="AJ55" s="53"/>
+      <c r="AK55" s="53"/>
+      <c r="AL55" s="53"/>
+      <c r="AM55" s="53"/>
+      <c r="AN55" s="53"/>
+      <c r="AO55" s="53"/>
+      <c r="AP55" s="53"/>
+      <c r="AQ55" s="53"/>
+      <c r="AR55" s="53"/>
+      <c r="AS55" s="53"/>
+      <c r="AT55" s="53"/>
+      <c r="AU55" s="53"/>
+      <c r="AV55" s="53"/>
+      <c r="AW55" s="53"/>
+      <c r="AX55" s="53"/>
+      <c r="AY55" s="53"/>
+      <c r="AZ55" s="53"/>
+      <c r="BA55" s="53"/>
+      <c r="BB55" s="53"/>
+    </row>
+    <row r="56" spans="1:66" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="8"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="106"/>
+      <c r="F56" s="106"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="99"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="9"/>
+      <c r="R56" s="9"/>
+      <c r="S56" s="9"/>
+      <c r="T56" s="9"/>
+      <c r="U56" s="9"/>
+      <c r="V56" s="9"/>
+      <c r="W56" s="9"/>
+      <c r="X56" s="9"/>
+      <c r="Y56" s="9"/>
+      <c r="Z56" s="9"/>
+      <c r="AA56" s="9"/>
+      <c r="AB56" s="9"/>
+      <c r="AC56" s="9"/>
+      <c r="AD56" s="9"/>
+      <c r="AE56" s="9"/>
+      <c r="AF56" s="9"/>
+      <c r="AG56" s="9"/>
+      <c r="AH56" s="9"/>
+      <c r="AI56" s="9"/>
+      <c r="AJ56" s="9"/>
+      <c r="AK56" s="9"/>
+      <c r="AL56" s="9"/>
+      <c r="AM56" s="9"/>
+      <c r="AN56" s="9"/>
+      <c r="AO56" s="9"/>
+      <c r="AP56" s="9"/>
+      <c r="AQ56" s="9"/>
+      <c r="AR56" s="9"/>
+      <c r="AS56" s="9"/>
+      <c r="AT56" s="9"/>
+      <c r="AU56" s="9"/>
+      <c r="AV56" s="9"/>
+      <c r="AW56" s="9"/>
+      <c r="AX56" s="9"/>
+      <c r="AY56" s="9"/>
+      <c r="AZ56" s="9"/>
+      <c r="BA56" s="9"/>
+      <c r="BB56" s="9"/>
+      <c r="BC56" s="9"/>
+      <c r="BD56" s="9"/>
+      <c r="BE56" s="9"/>
+      <c r="BF56" s="9"/>
+      <c r="BG56" s="9"/>
+      <c r="BH56" s="9"/>
+      <c r="BI56" s="9"/>
+      <c r="BJ56" s="9"/>
+      <c r="BK56" s="9"/>
+      <c r="BL56" s="9"/>
+      <c r="BM56" s="9"/>
+      <c r="BN56" s="9"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
     <mergeCell ref="BH5:BN5"/>
     <mergeCell ref="BA5:BG5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -6535,9 +6702,15 @@
     <mergeCell ref="AT4:AZ4"/>
     <mergeCell ref="AT5:AZ5"/>
     <mergeCell ref="AM4:AS4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H41:H48 H8:H32">
+  <conditionalFormatting sqref="H42:H49 H8:H33">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6556,7 +6729,7 @@
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN17 K22:BN48">
+  <conditionalFormatting sqref="K8:BN17 K22:BN49">
     <cfRule type="expression" dxfId="15" priority="56">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
@@ -6564,12 +6737,12 @@
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K41:BN48 K6:BN32">
+  <conditionalFormatting sqref="K42:BN49 K6:BN33">
     <cfRule type="expression" dxfId="13" priority="16">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33:H40">
+  <conditionalFormatting sqref="H34:H41">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6583,12 +6756,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33:BN40">
+  <conditionalFormatting sqref="K34:BN41">
     <cfRule type="expression" dxfId="12" priority="2">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49:BB54">
+  <conditionalFormatting sqref="E50:BB55">
     <cfRule type="expression" dxfId="11" priority="60">
       <formula>AND(#REF!&lt;=Q$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=Q$6)</formula>
     </cfRule>
@@ -6596,7 +6769,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=Q$6,#REF!&gt;=Q$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49:BB54">
+  <conditionalFormatting sqref="E50:BB55">
     <cfRule type="expression" dxfId="9" priority="63">
       <formula>Q$6=TODAY()</formula>
     </cfRule>
@@ -6625,7 +6798,7 @@
       <formula>AND(NOT(ISBLANK($E18)),$E18&lt;=K$6,$F20&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49:D54">
+  <conditionalFormatting sqref="A50:D55">
     <cfRule type="expression" dxfId="2" priority="78">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -6633,7 +6806,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49:D54">
+  <conditionalFormatting sqref="A50:D55">
     <cfRule type="expression" dxfId="0" priority="82">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -6648,7 +6821,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A47:B48 E47:H48 G17:H17 G27:H27 G41:H41 H21 H19 H28:H31 H42:H45" unlockedFormula="1"/>
+    <ignoredError sqref="A48:B49 E48:H49 G17:H17 G28:H28 G42:H42 H19 H29:H32 H43:H46" unlockedFormula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -6696,7 +6869,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H41:H48 H8:H32</xm:sqref>
+          <xm:sqref>H42:H49 H8:H33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{564E9A70-D213-4B59-9E35-13A2D63EE04B}">
@@ -6711,7 +6884,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H33:H40</xm:sqref>
+          <xm:sqref>H34:H41</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Updated sechdule with info related to plan,sequnce diagram
</commit_message>
<xml_diff>
--- a/Planning/CAR_Project_ Schedule.xlsx
+++ b/Planning/CAR_Project_ Schedule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatma\Desktop\CarPurchasing\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI_MATRIEL\project managment\project\CarPurchasing\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>WBS</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>Tue 5/07/2019</t>
+  </si>
+  <si>
+    <t>Tue 5/7/19</t>
   </si>
 </sst>
 </file>
@@ -1458,64 +1461,64 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="31" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="29" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="29" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="31" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1818,7 +1821,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1882,7 +1885,7 @@
                   <a14:compatExt spid="_x0000_s9262"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E200000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E200000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2077,6 +2080,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="AutoShape 9"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7972425" cy="8610600"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 9"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2406,7 +2457,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S27" sqref="S27"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2434,29 +2485,29 @@
       <c r="E1" s="94"/>
       <c r="F1" s="94"/>
       <c r="I1" s="74"/>
-      <c r="K1" s="120" t="s">
+      <c r="K1" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120"/>
-      <c r="Q1" s="120"/>
-      <c r="R1" s="120"/>
-      <c r="S1" s="120"/>
-      <c r="T1" s="120"/>
-      <c r="U1" s="120"/>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120"/>
-      <c r="X1" s="120"/>
-      <c r="Y1" s="120"/>
-      <c r="Z1" s="120"/>
-      <c r="AA1" s="120"/>
-      <c r="AB1" s="120"/>
-      <c r="AC1" s="120"/>
-      <c r="AD1" s="120"/>
-      <c r="AE1" s="120"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="118"/>
+      <c r="V1" s="118"/>
+      <c r="W1" s="118"/>
+      <c r="X1" s="118"/>
+      <c r="Y1" s="118"/>
+      <c r="Z1" s="118"/>
+      <c r="AA1" s="118"/>
+      <c r="AB1" s="118"/>
+      <c r="AC1" s="118"/>
+      <c r="AD1" s="118"/>
+      <c r="AE1" s="118"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
@@ -2501,11 +2552,11 @@
       <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="114">
+      <c r="C4" s="128">
         <v>43582</v>
       </c>
-      <c r="D4" s="114"/>
-      <c r="E4" s="114"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
       <c r="F4" s="108"/>
       <c r="G4" s="59" t="s">
         <v>7</v>
@@ -2515,170 +2566,170 @@
       </c>
       <c r="I4" s="57"/>
       <c r="J4" s="16"/>
-      <c r="K4" s="111" t="str">
+      <c r="K4" s="119" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="111" t="str">
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="120"/>
+      <c r="O4" s="120"/>
+      <c r="P4" s="120"/>
+      <c r="Q4" s="121"/>
+      <c r="R4" s="119" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="113"/>
-      <c r="Y4" s="111" t="str">
+      <c r="S4" s="120"/>
+      <c r="T4" s="120"/>
+      <c r="U4" s="120"/>
+      <c r="V4" s="120"/>
+      <c r="W4" s="120"/>
+      <c r="X4" s="121"/>
+      <c r="Y4" s="119" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="112"/>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="112"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="112"/>
-      <c r="AE4" s="113"/>
-      <c r="AF4" s="111" t="str">
+      <c r="Z4" s="120"/>
+      <c r="AA4" s="120"/>
+      <c r="AB4" s="120"/>
+      <c r="AC4" s="120"/>
+      <c r="AD4" s="120"/>
+      <c r="AE4" s="121"/>
+      <c r="AF4" s="119" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="112"/>
-      <c r="AH4" s="112"/>
-      <c r="AI4" s="112"/>
-      <c r="AJ4" s="112"/>
-      <c r="AK4" s="112"/>
-      <c r="AL4" s="113"/>
-      <c r="AM4" s="111" t="str">
+      <c r="AG4" s="120"/>
+      <c r="AH4" s="120"/>
+      <c r="AI4" s="120"/>
+      <c r="AJ4" s="120"/>
+      <c r="AK4" s="120"/>
+      <c r="AL4" s="121"/>
+      <c r="AM4" s="119" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="112"/>
-      <c r="AO4" s="112"/>
-      <c r="AP4" s="112"/>
-      <c r="AQ4" s="112"/>
-      <c r="AR4" s="112"/>
-      <c r="AS4" s="113"/>
-      <c r="AT4" s="111" t="str">
+      <c r="AN4" s="120"/>
+      <c r="AO4" s="120"/>
+      <c r="AP4" s="120"/>
+      <c r="AQ4" s="120"/>
+      <c r="AR4" s="120"/>
+      <c r="AS4" s="121"/>
+      <c r="AT4" s="119" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="112"/>
-      <c r="AV4" s="112"/>
-      <c r="AW4" s="112"/>
-      <c r="AX4" s="112"/>
-      <c r="AY4" s="112"/>
-      <c r="AZ4" s="121"/>
-      <c r="BA4" s="119"/>
-      <c r="BB4" s="119"/>
-      <c r="BC4" s="119"/>
-      <c r="BD4" s="119"/>
-      <c r="BE4" s="119"/>
-      <c r="BF4" s="119"/>
-      <c r="BG4" s="119"/>
-      <c r="BH4" s="119"/>
-      <c r="BI4" s="119"/>
-      <c r="BJ4" s="119"/>
-      <c r="BK4" s="119"/>
-      <c r="BL4" s="119"/>
-      <c r="BM4" s="119"/>
-      <c r="BN4" s="119"/>
+      <c r="AU4" s="120"/>
+      <c r="AV4" s="120"/>
+      <c r="AW4" s="120"/>
+      <c r="AX4" s="120"/>
+      <c r="AY4" s="120"/>
+      <c r="AZ4" s="125"/>
+      <c r="BA4" s="117"/>
+      <c r="BB4" s="117"/>
+      <c r="BC4" s="117"/>
+      <c r="BD4" s="117"/>
+      <c r="BE4" s="117"/>
+      <c r="BF4" s="117"/>
+      <c r="BG4" s="117"/>
+      <c r="BH4" s="117"/>
+      <c r="BI4" s="117"/>
+      <c r="BJ4" s="117"/>
+      <c r="BK4" s="117"/>
+      <c r="BL4" s="117"/>
+      <c r="BM4" s="117"/>
+      <c r="BN4" s="117"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="56"/>
       <c r="B5" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="110" t="s">
+      <c r="C5" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="127"/>
       <c r="F5" s="109"/>
       <c r="G5" s="58"/>
       <c r="H5" s="95"/>
       <c r="I5" s="58"/>
       <c r="J5" s="16"/>
-      <c r="K5" s="115">
+      <c r="K5" s="122">
         <f>K6</f>
         <v>43577</v>
       </c>
-      <c r="L5" s="116"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="117"/>
-      <c r="R5" s="115">
+      <c r="L5" s="123"/>
+      <c r="M5" s="123"/>
+      <c r="N5" s="123"/>
+      <c r="O5" s="123"/>
+      <c r="P5" s="123"/>
+      <c r="Q5" s="124"/>
+      <c r="R5" s="122">
         <f>R6</f>
         <v>43584</v>
       </c>
-      <c r="S5" s="116"/>
-      <c r="T5" s="116"/>
-      <c r="U5" s="116"/>
-      <c r="V5" s="116"/>
-      <c r="W5" s="116"/>
-      <c r="X5" s="117"/>
-      <c r="Y5" s="115">
+      <c r="S5" s="123"/>
+      <c r="T5" s="123"/>
+      <c r="U5" s="123"/>
+      <c r="V5" s="123"/>
+      <c r="W5" s="123"/>
+      <c r="X5" s="124"/>
+      <c r="Y5" s="122">
         <f>Y6</f>
         <v>43591</v>
       </c>
-      <c r="Z5" s="116"/>
-      <c r="AA5" s="116"/>
-      <c r="AB5" s="116"/>
-      <c r="AC5" s="116"/>
-      <c r="AD5" s="116"/>
-      <c r="AE5" s="117"/>
-      <c r="AF5" s="115">
+      <c r="Z5" s="123"/>
+      <c r="AA5" s="123"/>
+      <c r="AB5" s="123"/>
+      <c r="AC5" s="123"/>
+      <c r="AD5" s="123"/>
+      <c r="AE5" s="124"/>
+      <c r="AF5" s="122">
         <f>AF6</f>
         <v>43598</v>
       </c>
-      <c r="AG5" s="116"/>
-      <c r="AH5" s="116"/>
-      <c r="AI5" s="116"/>
-      <c r="AJ5" s="116"/>
-      <c r="AK5" s="116"/>
-      <c r="AL5" s="117"/>
-      <c r="AM5" s="115">
+      <c r="AG5" s="123"/>
+      <c r="AH5" s="123"/>
+      <c r="AI5" s="123"/>
+      <c r="AJ5" s="123"/>
+      <c r="AK5" s="123"/>
+      <c r="AL5" s="124"/>
+      <c r="AM5" s="122">
         <f>AM6</f>
         <v>43605</v>
       </c>
-      <c r="AN5" s="116"/>
-      <c r="AO5" s="116"/>
-      <c r="AP5" s="116"/>
-      <c r="AQ5" s="116"/>
-      <c r="AR5" s="116"/>
-      <c r="AS5" s="117"/>
-      <c r="AT5" s="115">
+      <c r="AN5" s="123"/>
+      <c r="AO5" s="123"/>
+      <c r="AP5" s="123"/>
+      <c r="AQ5" s="123"/>
+      <c r="AR5" s="123"/>
+      <c r="AS5" s="124"/>
+      <c r="AT5" s="122">
         <f>AT6</f>
         <v>43612</v>
       </c>
-      <c r="AU5" s="116"/>
-      <c r="AV5" s="116"/>
-      <c r="AW5" s="116"/>
-      <c r="AX5" s="116"/>
-      <c r="AY5" s="116"/>
-      <c r="AZ5" s="122"/>
-      <c r="BA5" s="118"/>
-      <c r="BB5" s="118"/>
-      <c r="BC5" s="118"/>
-      <c r="BD5" s="118"/>
-      <c r="BE5" s="118"/>
-      <c r="BF5" s="118"/>
-      <c r="BG5" s="118"/>
-      <c r="BH5" s="118"/>
-      <c r="BI5" s="118"/>
-      <c r="BJ5" s="118"/>
-      <c r="BK5" s="118"/>
-      <c r="BL5" s="118"/>
-      <c r="BM5" s="118"/>
-      <c r="BN5" s="118"/>
+      <c r="AU5" s="123"/>
+      <c r="AV5" s="123"/>
+      <c r="AW5" s="123"/>
+      <c r="AX5" s="123"/>
+      <c r="AY5" s="123"/>
+      <c r="AZ5" s="126"/>
+      <c r="BA5" s="116"/>
+      <c r="BB5" s="116"/>
+      <c r="BC5" s="116"/>
+      <c r="BD5" s="116"/>
+      <c r="BE5" s="116"/>
+      <c r="BF5" s="116"/>
+      <c r="BG5" s="116"/>
+      <c r="BH5" s="116"/>
+      <c r="BI5" s="116"/>
+      <c r="BJ5" s="116"/>
+      <c r="BK5" s="116"/>
+      <c r="BL5" s="116"/>
+      <c r="BM5" s="116"/>
+      <c r="BN5" s="116"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="15"/>
@@ -4095,8 +4146,8 @@
       <c r="R20" s="53"/>
       <c r="S20" s="53"/>
       <c r="T20" s="53"/>
-      <c r="U20" s="123"/>
-      <c r="V20" s="123"/>
+      <c r="U20" s="110"/>
+      <c r="V20" s="110"/>
       <c r="W20" s="53"/>
       <c r="X20" s="53"/>
       <c r="Y20" s="53"/>
@@ -4321,10 +4372,18 @@
         <v>57</v>
       </c>
       <c r="D23" s="72"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="29"/>
+      <c r="E23" s="98" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="28">
+        <v>2</v>
+      </c>
+      <c r="H23" s="29">
+        <v>1</v>
+      </c>
       <c r="I23" s="30"/>
       <c r="J23" s="47"/>
       <c r="K23" s="53"/>
@@ -4395,10 +4454,18 @@
         <v>28</v>
       </c>
       <c r="D24" s="72"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="29"/>
+      <c r="E24" s="98" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="28">
+        <v>2</v>
+      </c>
+      <c r="H24" s="29">
+        <v>1</v>
+      </c>
       <c r="I24" s="30"/>
       <c r="J24" s="47"/>
       <c r="K24" s="53"/>
@@ -4469,10 +4536,18 @@
         <v>57</v>
       </c>
       <c r="D25" s="72"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="29"/>
+      <c r="E25" s="98">
+        <v>43590</v>
+      </c>
+      <c r="F25" s="98">
+        <v>43591</v>
+      </c>
+      <c r="G25" s="28">
+        <v>2</v>
+      </c>
+      <c r="H25" s="29">
+        <v>1</v>
+      </c>
       <c r="I25" s="30"/>
       <c r="J25" s="47"/>
       <c r="K25" s="53"/>
@@ -4543,10 +4618,18 @@
         <v>57</v>
       </c>
       <c r="D26" s="72"/>
-      <c r="E26" s="98"/>
-      <c r="F26" s="98"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="29"/>
+      <c r="E26" s="98">
+        <v>43593</v>
+      </c>
+      <c r="F26" s="98">
+        <v>43595</v>
+      </c>
+      <c r="G26" s="28">
+        <v>1</v>
+      </c>
+      <c r="H26" s="29">
+        <v>10</v>
+      </c>
       <c r="I26" s="30"/>
       <c r="J26" s="47"/>
       <c r="K26" s="53"/>
@@ -4616,23 +4699,23 @@
       <c r="C27" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="124"/>
-      <c r="E27" s="125" t="s">
+      <c r="D27" s="111"/>
+      <c r="E27" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="125" t="s">
+      <c r="F27" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="G27" s="126">
+      <c r="G27" s="113">
         <v>1</v>
       </c>
       <c r="H27" s="29">
         <v>1</v>
       </c>
-      <c r="I27" s="127">
+      <c r="I27" s="114">
         <v>1</v>
       </c>
-      <c r="J27" s="128"/>
+      <c r="J27" s="115"/>
       <c r="K27" s="53"/>
       <c r="L27" s="53"/>
       <c r="M27" s="53"/>
@@ -4641,7 +4724,7 @@
       <c r="P27" s="53"/>
       <c r="Q27" s="53"/>
       <c r="R27" s="53"/>
-      <c r="S27" s="123"/>
+      <c r="S27" s="110"/>
       <c r="T27" s="53"/>
       <c r="U27" s="53"/>
       <c r="V27" s="53"/>
@@ -6689,6 +6772,12 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
     <mergeCell ref="BH5:BN5"/>
     <mergeCell ref="BA5:BG5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -6702,12 +6791,6 @@
     <mergeCell ref="AT4:AZ4"/>
     <mergeCell ref="AT5:AZ5"/>
     <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H42:H49 H8:H33">

</xml_diff>